<commit_message>
Re writing the methods
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Documents\WCU\thesisschmesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA28A92-E21D-4B1D-B250-88805EC5F4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4B91D3-D7B9-4B30-B73B-C6ACFA1C1EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="58">
   <si>
     <t>Transect</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>NE</t>
-  </si>
-  <si>
-    <t>Alnus</t>
   </si>
   <si>
     <t>Rubus</t>
@@ -225,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +237,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +258,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -264,10 +273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -298,8 +308,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1370,9 +1393,6 @@
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Alnus</c:v>
-                      </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -1402,7 +1422,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-5B1A-484F-A519-22E9686ADB27}"/>
                   </c:ext>
@@ -2747,7 +2767,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ground Cover'!$E$1</c15:sqref>
@@ -2756,9 +2776,6 @@
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Alnus</c:v>
-                      </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:tx>
@@ -2775,7 +2792,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ground Cover'!$E$24:$E$43</c15:sqref>
@@ -2788,7 +2805,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-AF08-472E-A535-5AE451D7C914}"/>
                   </c:ext>
@@ -8433,8 +8450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6DF77C-F4C9-40DD-B173-895D836B5FA9}">
   <dimension ref="A1:AG103"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F61" sqref="F1:F1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8470,13 +8487,13 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -8485,7 +8502,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -8530,43 +8547,43 @@
         <v>11</v>
       </c>
       <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" t="s">
-        <v>36</v>
-      </c>
       <c r="AG1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -8610,7 +8627,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" ref="N2:N33" si="0">AVERAGE(O2:R2)</f>
+        <f>AVERAGE(O2:R2)</f>
         <v>20.7</v>
       </c>
       <c r="O2" s="2">
@@ -8685,7 +8702,7 @@
         <v>17</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O3:R3)</f>
         <v>12.45</v>
       </c>
       <c r="O3" s="2">
@@ -8716,7 +8733,7 @@
         <v>25</v>
       </c>
       <c r="AG3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -8760,7 +8777,7 @@
         <v>17</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O4:R4)</f>
         <v>13.3</v>
       </c>
       <c r="O4" s="2">
@@ -8835,7 +8852,7 @@
         <v>17</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O5:R5)</f>
         <v>9.8749999999999982</v>
       </c>
       <c r="O5" s="2">
@@ -8901,7 +8918,7 @@
         <v>17</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O6:R6)</f>
         <v>8.8249999999999993</v>
       </c>
       <c r="O6" s="2">
@@ -8979,7 +8996,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O7:R7)</f>
         <v>13.024999999999999</v>
       </c>
       <c r="O7" s="2">
@@ -9013,7 +9030,7 @@
         <v>1</v>
       </c>
       <c r="AG7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
@@ -9057,7 +9074,7 @@
         <v>17</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O8:R8)</f>
         <v>13.15</v>
       </c>
       <c r="O8" s="2">
@@ -9129,7 +9146,7 @@
         <v>17</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O9:R9)</f>
         <v>14</v>
       </c>
       <c r="O9" s="2">
@@ -9201,7 +9218,7 @@
         <v>17</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O10:R10)</f>
         <v>12.774999999999999</v>
       </c>
       <c r="O10" s="2">
@@ -9276,7 +9293,7 @@
         <v>17</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O11:R11)</f>
         <v>14.425000000000001</v>
       </c>
       <c r="O11" s="2">
@@ -9351,7 +9368,7 @@
         <v>17</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O12:R12)</f>
         <v>16.849999999999998</v>
       </c>
       <c r="O12" s="2">
@@ -9420,7 +9437,7 @@
         <v>17</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O13:R13)</f>
         <v>20.074999999999999</v>
       </c>
       <c r="O13" s="2">
@@ -9489,7 +9506,7 @@
         <v>17</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O14:R14)</f>
         <v>24.375</v>
       </c>
       <c r="O14" s="2">
@@ -9561,7 +9578,7 @@
         <v>17</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O15:R15)</f>
         <v>19.95</v>
       </c>
       <c r="O15" s="2">
@@ -9636,7 +9653,7 @@
         <v>17</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O16:R16)</f>
         <v>13.8</v>
       </c>
       <c r="O16" s="2">
@@ -9714,7 +9731,7 @@
         <v>17</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O17:R17)</f>
         <v>12.675000000000001</v>
       </c>
       <c r="O17" s="2">
@@ -9789,7 +9806,7 @@
         <v>17</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O18:R18)</f>
         <v>16.2</v>
       </c>
       <c r="O18" s="2">
@@ -9861,7 +9878,7 @@
         <v>17</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O19:R19)</f>
         <v>16.150000000000002</v>
       </c>
       <c r="O19" s="2">
@@ -9933,7 +9950,7 @@
         <v>17</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O20:R20)</f>
         <v>12.425000000000001</v>
       </c>
       <c r="O20" s="2">
@@ -10005,7 +10022,7 @@
         <v>17</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O21:R21)</f>
         <v>16.724999999999998</v>
       </c>
       <c r="O21" s="2">
@@ -10077,7 +10094,7 @@
         <v>17</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O22:R22)</f>
         <v>16.424999999999997</v>
       </c>
       <c r="O22" s="2">
@@ -10149,7 +10166,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O23:R23)</f>
         <v>12.725000000000001</v>
       </c>
       <c r="O23" s="2">
@@ -10221,7 +10238,7 @@
         <v>19</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O24:R24)</f>
         <v>12.25</v>
       </c>
       <c r="O24" s="2">
@@ -10290,7 +10307,7 @@
         <v>19</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O25:R25)</f>
         <v>10.6</v>
       </c>
       <c r="O25" s="2">
@@ -10359,7 +10376,7 @@
         <v>19</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O26:R26)</f>
         <v>16.125</v>
       </c>
       <c r="O26" s="2">
@@ -10428,7 +10445,7 @@
         <v>19</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O27:R27)</f>
         <v>8.3250000000000011</v>
       </c>
       <c r="O27" s="2">
@@ -10459,7 +10476,7 @@
         <v>17</v>
       </c>
       <c r="AG27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
@@ -10503,7 +10520,7 @@
         <v>19</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O28:R28)</f>
         <v>10.700000000000001</v>
       </c>
       <c r="O28" s="2">
@@ -10581,7 +10598,7 @@
         <v>17</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O29:R29)</f>
         <v>26.2</v>
       </c>
       <c r="O29" s="2">
@@ -10662,7 +10679,7 @@
         <v>17</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O30:R30)</f>
         <v>20.725000000000001</v>
       </c>
       <c r="O30" s="2">
@@ -10731,7 +10748,7 @@
         <v>17</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O31:R31)</f>
         <v>13.675000000000001</v>
       </c>
       <c r="O31" s="2">
@@ -10803,7 +10820,7 @@
         <v>17</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O32:R32)</f>
         <v>21.625</v>
       </c>
       <c r="O32" s="2">
@@ -10872,7 +10889,7 @@
         <v>17</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(O33:R33)</f>
         <v>16.75</v>
       </c>
       <c r="O33" s="2">
@@ -10944,7 +10961,7 @@
         <v>17</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" ref="N34:N65" si="1">AVERAGE(O34:R34)</f>
+        <f>AVERAGE(O34:R34)</f>
         <v>16.074999999999999</v>
       </c>
       <c r="O34" s="2">
@@ -11013,7 +11030,7 @@
         <v>17</v>
       </c>
       <c r="N35" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O35:R35)</f>
         <v>8</v>
       </c>
       <c r="O35" s="2">
@@ -11085,7 +11102,7 @@
         <v>17</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O36:R36)</f>
         <v>10.25</v>
       </c>
       <c r="O36" s="2">
@@ -11160,7 +11177,7 @@
         <v>17</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O37:R37)</f>
         <v>10.225</v>
       </c>
       <c r="O37" s="2">
@@ -11232,7 +11249,7 @@
         <v>17</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O38:R38)</f>
         <v>15.4</v>
       </c>
       <c r="O38" s="2">
@@ -11304,7 +11321,7 @@
         <v>17</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O39:R39)</f>
         <v>10.85</v>
       </c>
       <c r="O39" s="2">
@@ -11376,7 +11393,7 @@
         <v>17</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O40:R40)</f>
         <v>12.8</v>
       </c>
       <c r="O40" s="2">
@@ -11451,7 +11468,7 @@
         <v>17</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O41:R41)</f>
         <v>12.924999999999999</v>
       </c>
       <c r="O41" s="2">
@@ -11520,7 +11537,7 @@
         <v>17</v>
       </c>
       <c r="N42" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O42:R42)</f>
         <v>15.975</v>
       </c>
       <c r="O42" s="2">
@@ -11598,7 +11615,7 @@
         <v>17</v>
       </c>
       <c r="N43" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O43:R43)</f>
         <v>11.75</v>
       </c>
       <c r="O43" s="2">
@@ -11670,7 +11687,7 @@
         <v>19</v>
       </c>
       <c r="N44" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O44:R44)</f>
         <v>18.675000000000001</v>
       </c>
       <c r="O44" s="2">
@@ -11739,7 +11756,7 @@
         <v>19</v>
       </c>
       <c r="N45" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O45:R45)</f>
         <v>16.3</v>
       </c>
       <c r="O45" s="2">
@@ -11808,7 +11825,7 @@
         <v>19</v>
       </c>
       <c r="N46" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O46:R46)</f>
         <v>15.274999999999999</v>
       </c>
       <c r="O46" s="2">
@@ -11854,7 +11871,7 @@
         <v>6</v>
       </c>
       <c r="AG46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
@@ -11898,7 +11915,7 @@
         <v>17</v>
       </c>
       <c r="N47" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O47:R47)</f>
         <v>14</v>
       </c>
       <c r="O47" s="2">
@@ -11973,7 +11990,7 @@
         <v>17</v>
       </c>
       <c r="N48" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O48:R48)</f>
         <v>6.5</v>
       </c>
       <c r="O48" s="2">
@@ -12048,7 +12065,7 @@
         <v>17</v>
       </c>
       <c r="N49" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O49:R49)</f>
         <v>5.25</v>
       </c>
       <c r="O49" s="2">
@@ -12126,7 +12143,7 @@
         <v>17</v>
       </c>
       <c r="N50" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O50:R50)</f>
         <v>16.575000000000003</v>
       </c>
       <c r="O50" s="2">
@@ -12198,7 +12215,7 @@
         <v>17</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O51:R51)</f>
         <v>13.875</v>
       </c>
       <c r="O51" s="2">
@@ -12273,7 +12290,7 @@
         <v>17</v>
       </c>
       <c r="N52" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O52:R52)</f>
         <v>11.525</v>
       </c>
       <c r="O52" s="2">
@@ -12342,7 +12359,7 @@
         <v>17</v>
       </c>
       <c r="N53" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O53:R53)</f>
         <v>12.9</v>
       </c>
       <c r="O53" s="2">
@@ -12414,7 +12431,7 @@
         <v>17</v>
       </c>
       <c r="N54" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O54:R54)</f>
         <v>15.225</v>
       </c>
       <c r="O54" s="2">
@@ -12486,7 +12503,7 @@
         <v>17</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O55:R55)</f>
         <v>19.675000000000001</v>
       </c>
       <c r="O55" s="2">
@@ -12555,7 +12572,7 @@
         <v>17</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O56:R56)</f>
         <v>19.899999999999999</v>
       </c>
       <c r="O56" s="2">
@@ -12633,7 +12650,7 @@
         <v>17</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O57:R57)</f>
         <v>17.275000000000002</v>
       </c>
       <c r="O57" s="2">
@@ -12708,7 +12725,7 @@
         <v>17</v>
       </c>
       <c r="N58" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O58:R58)</f>
         <v>19.625</v>
       </c>
       <c r="O58" s="2">
@@ -12783,7 +12800,7 @@
         <v>17</v>
       </c>
       <c r="N59" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O59:R59)</f>
         <v>10.75</v>
       </c>
       <c r="O59" s="2">
@@ -12858,7 +12875,7 @@
         <v>17</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O60:R60)</f>
         <v>8.9499999999999993</v>
       </c>
       <c r="O60" s="2">
@@ -12936,7 +12953,7 @@
         <v>17</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O61:R61)</f>
         <v>20.524999999999999</v>
       </c>
       <c r="O61" s="2">
@@ -13011,7 +13028,7 @@
         <v>17</v>
       </c>
       <c r="N62" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O62:R62)</f>
         <v>19.45</v>
       </c>
       <c r="O62" s="2">
@@ -13077,7 +13094,7 @@
         <v>17</v>
       </c>
       <c r="N63" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O63:R63)</f>
         <v>13.524999999999999</v>
       </c>
       <c r="O63" s="2">
@@ -13146,7 +13163,7 @@
         <v>17</v>
       </c>
       <c r="N64" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O64:R64)</f>
         <v>13.375</v>
       </c>
       <c r="O64" s="2">
@@ -13218,7 +13235,7 @@
         <v>17</v>
       </c>
       <c r="N65" s="2">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(O65:R65)</f>
         <v>14.399999999999999</v>
       </c>
       <c r="O65" s="2">
@@ -13287,7 +13304,7 @@
         <v>17</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" ref="N66:N97" si="2">AVERAGE(O66:R66)</f>
+        <f>AVERAGE(O66:R66)</f>
         <v>11.675000000000001</v>
       </c>
       <c r="O66" s="2">
@@ -13359,7 +13376,7 @@
         <v>17</v>
       </c>
       <c r="N67" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O67:R67)</f>
         <v>18.149999999999999</v>
       </c>
       <c r="O67" s="2">
@@ -13431,7 +13448,7 @@
         <v>17</v>
       </c>
       <c r="N68" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O68:R68)</f>
         <v>20.175000000000001</v>
       </c>
       <c r="O68" s="2">
@@ -13500,7 +13517,7 @@
         <v>19</v>
       </c>
       <c r="N69" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O69:R69)</f>
         <v>15.475</v>
       </c>
       <c r="O69" s="2">
@@ -13569,7 +13586,7 @@
         <v>19</v>
       </c>
       <c r="N70" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O70:R70)</f>
         <v>15.125</v>
       </c>
       <c r="O70" s="2">
@@ -13644,7 +13661,7 @@
         <v>19</v>
       </c>
       <c r="N71" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O71:R71)</f>
         <v>11.5</v>
       </c>
       <c r="O71" s="2">
@@ -13719,7 +13736,7 @@
         <v>19</v>
       </c>
       <c r="N72" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O72:R72)</f>
         <v>9.0749999999999993</v>
       </c>
       <c r="O72" s="2">
@@ -13791,7 +13808,7 @@
         <v>19</v>
       </c>
       <c r="N73" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O73:R73)</f>
         <v>15.05</v>
       </c>
       <c r="O73" s="2">
@@ -13866,7 +13883,7 @@
         <v>19</v>
       </c>
       <c r="N74" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O74:R74)</f>
         <v>17.049999999999997</v>
       </c>
       <c r="O74" s="2">
@@ -13941,7 +13958,7 @@
         <v>19</v>
       </c>
       <c r="N75" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O75:R75)</f>
         <v>13.674999999999999</v>
       </c>
       <c r="O75" s="2">
@@ -14010,7 +14027,7 @@
         <v>19</v>
       </c>
       <c r="N76" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O76:R76)</f>
         <v>14.700000000000001</v>
       </c>
       <c r="O76" s="2">
@@ -14079,7 +14096,7 @@
         <v>19</v>
       </c>
       <c r="N77" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O77:R77)</f>
         <v>17.625</v>
       </c>
       <c r="O77" s="2">
@@ -14113,7 +14130,7 @@
         <v>12</v>
       </c>
       <c r="AG77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
@@ -14157,7 +14174,7 @@
         <v>19</v>
       </c>
       <c r="N78" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O78:R78)</f>
         <v>11.575000000000001</v>
       </c>
       <c r="O78" s="2">
@@ -14232,7 +14249,7 @@
         <v>19</v>
       </c>
       <c r="N79" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O79:R79)</f>
         <v>15.175000000000001</v>
       </c>
       <c r="O79" s="2">
@@ -14310,7 +14327,7 @@
         <v>19</v>
       </c>
       <c r="N80" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O80:R80)</f>
         <v>12.025</v>
       </c>
       <c r="O80" s="2">
@@ -14379,7 +14396,7 @@
         <v>19</v>
       </c>
       <c r="N81" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O81:R81)</f>
         <v>5.6750000000000007</v>
       </c>
       <c r="O81" s="2">
@@ -14410,7 +14427,7 @@
         <v>2</v>
       </c>
       <c r="AG81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.25">
@@ -14454,7 +14471,7 @@
         <v>19</v>
       </c>
       <c r="N82" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O82:R82)</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="O82" s="2">
@@ -14529,7 +14546,7 @@
         <v>19</v>
       </c>
       <c r="N83" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O83:R83)</f>
         <v>10.225</v>
       </c>
       <c r="O83" s="2">
@@ -14607,7 +14624,7 @@
         <v>19</v>
       </c>
       <c r="N84" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O84:R84)</f>
         <v>13.899999999999999</v>
       </c>
       <c r="O84" s="2">
@@ -14685,7 +14702,7 @@
         <v>19</v>
       </c>
       <c r="N85" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O85:R85)</f>
         <v>11.1</v>
       </c>
       <c r="O85" s="2">
@@ -14766,7 +14783,7 @@
         <v>19</v>
       </c>
       <c r="N86" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O86:R86)</f>
         <v>8.0250000000000004</v>
       </c>
       <c r="O86" s="2">
@@ -14835,7 +14852,7 @@
         <v>19</v>
       </c>
       <c r="N87" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O87:R87)</f>
         <v>12.9</v>
       </c>
       <c r="O87" s="2">
@@ -14875,7 +14892,7 @@
         <v>2</v>
       </c>
       <c r="AG87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.25">
@@ -14919,7 +14936,7 @@
         <v>17</v>
       </c>
       <c r="N88" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O88:R88)</f>
         <v>11.074999999999999</v>
       </c>
       <c r="O88" s="2">
@@ -14991,7 +15008,7 @@
         <v>17</v>
       </c>
       <c r="N89" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O89:R89)</f>
         <v>13.65</v>
       </c>
       <c r="O89" s="2">
@@ -15063,7 +15080,7 @@
         <v>17</v>
       </c>
       <c r="N90" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O90:R90)</f>
         <v>14</v>
       </c>
       <c r="O90" s="2">
@@ -15138,7 +15155,7 @@
         <v>17</v>
       </c>
       <c r="N91" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O91:R91)</f>
         <v>18.350000000000001</v>
       </c>
       <c r="O91" s="2">
@@ -15213,7 +15230,7 @@
         <v>17</v>
       </c>
       <c r="N92" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O92:R92)</f>
         <v>19.125</v>
       </c>
       <c r="O92" s="2">
@@ -15285,7 +15302,7 @@
         <v>17</v>
       </c>
       <c r="N93" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O93:R93)</f>
         <v>14.425000000000001</v>
       </c>
       <c r="O93" s="2">
@@ -15363,7 +15380,7 @@
         <v>17</v>
       </c>
       <c r="N94" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O94:R94)</f>
         <v>14.850000000000001</v>
       </c>
       <c r="O94" s="2">
@@ -15432,7 +15449,7 @@
         <v>17</v>
       </c>
       <c r="N95" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O95:R95)</f>
         <v>16.850000000000001</v>
       </c>
       <c r="O95" s="2">
@@ -15507,7 +15524,7 @@
         <v>17</v>
       </c>
       <c r="N96" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O96:R96)</f>
         <v>11.125</v>
       </c>
       <c r="O96" s="2">
@@ -15582,7 +15599,7 @@
         <v>17</v>
       </c>
       <c r="N97" s="2">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(O97:R97)</f>
         <v>11.15</v>
       </c>
       <c r="O97" s="2">
@@ -15663,7 +15680,7 @@
         <v>17</v>
       </c>
       <c r="N98" s="2">
-        <f t="shared" ref="N98:N100" si="3">AVERAGE(O98:R98)</f>
+        <f>AVERAGE(O98:R98)</f>
         <v>16.600000000000001</v>
       </c>
       <c r="O98" s="2">
@@ -15732,7 +15749,7 @@
         <v>17</v>
       </c>
       <c r="N99" s="2">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(O99:R99)</f>
         <v>9.7000000000000011</v>
       </c>
       <c r="O99" s="2">
@@ -15804,7 +15821,7 @@
         <v>17</v>
       </c>
       <c r="N100" s="2">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(O100:R100)</f>
         <v>14.274999999999999</v>
       </c>
       <c r="O100" s="2">
@@ -15854,7 +15871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA563366-8DA0-4A43-8949-852B034D9918}">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
@@ -15890,49 +15907,46 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
       <c r="R1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -15987,7 +16001,7 @@
         <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -16100,7 +16114,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -16626,7 +16640,7 @@
         <v>17</v>
       </c>
       <c r="R27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -17144,7 +17158,7 @@
         <v>6</v>
       </c>
       <c r="R46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -17977,7 +17991,7 @@
         <v>12</v>
       </c>
       <c r="R77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -18090,7 +18104,7 @@
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
@@ -18273,7 +18287,7 @@
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
@@ -18660,28 +18674,28 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -18692,13 +18706,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5">
         <v>3.23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -18714,13 +18728,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5">
         <v>3.4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -18736,7 +18750,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -18754,13 +18768,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5">
         <v>1.6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -18776,13 +18790,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5">
         <v>4.8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -18798,13 +18812,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="5">
         <v>2.7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5">
         <v>6</v>
@@ -18820,13 +18834,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5">
         <v>2.14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="5">
         <v>7</v>
@@ -18842,13 +18856,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5">
         <v>3.8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="5">
         <v>8</v>
@@ -18864,7 +18878,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -18882,13 +18896,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5">
         <v>3.7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -18904,13 +18918,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5">
         <v>3.1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="5">
         <v>11</v>
@@ -18926,19 +18940,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5">
         <v>4.18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5">
         <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="7">
         <v>44759</v>
@@ -18952,19 +18966,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5">
         <v>4.24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="5">
         <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="7">
         <v>44759</v>
@@ -18978,19 +18992,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5">
         <v>2.8</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="5">
         <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="7">
         <v>44764</v>
@@ -19004,19 +19018,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5">
         <v>4.17</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="5">
         <v>15</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="7">
         <v>44759</v>
@@ -19030,19 +19044,19 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5">
         <v>1.21</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="5">
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="7">
         <v>44767</v>
@@ -19056,19 +19070,19 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="5">
         <v>1.1299999999999999</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5">
         <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="7">
         <v>44767</v>
@@ -19082,7 +19096,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -19100,7 +19114,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -19118,13 +19132,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="8">
         <v>1.1000000000000001</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="5">
         <v>20</v>
@@ -19140,19 +19154,19 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5">
         <v>4.13</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="5">
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="7">
         <v>44767</v>
@@ -19166,7 +19180,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -19184,13 +19198,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5">
         <v>4.3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="5">
         <v>23</v>
@@ -19206,13 +19220,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="5">
         <v>2.16</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5">
         <v>24</v>
@@ -19228,13 +19242,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5">
         <v>4.16</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="5">
         <v>25</v>
@@ -19250,7 +19264,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -19268,19 +19282,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="5">
         <v>1.22</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="5">
         <v>27</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="7">
         <v>44759</v>
@@ -19294,19 +19308,19 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="8">
         <v>2.2000000000000002</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="5">
         <v>28</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" s="7">
         <v>44760</v>
@@ -19320,19 +19334,19 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="5">
         <v>1.1599999999999999</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="5">
         <v>29</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F30" s="7">
         <v>44762</v>
@@ -19346,13 +19360,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="5">
         <v>1.7</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="5">
         <v>30</v>
@@ -19375,8 +19389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70826AB2-0F3B-43B6-8E74-FD8F1FFA7EF4}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19387,164 +19401,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="5">
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="5">
         <v>3.23</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="5">
+      <c r="H3" s="6"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="15">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="15">
         <v>1.21</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="5">
+      <c r="M3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="15">
         <v>16</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="7">
+      <c r="O3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="16">
         <v>44767</v>
       </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="5">
         <v>3.4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="5">
         <v>2</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="5">
+      <c r="H4" s="6"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="15">
         <v>7</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="15">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="M4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="5">
+      <c r="N4" s="15">
         <v>17</v>
       </c>
-      <c r="O4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" s="7">
+      <c r="O4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="16">
         <v>44767</v>
       </c>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5">
         <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -19552,12 +19568,13 @@
         <v>3</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="I5" s="9"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="5">
         <v>30</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -19566,32 +19583,33 @@
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5">
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="5">
         <v>1.6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="5">
         <v>26</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -19600,112 +19618,115 @@
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5">
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="5">
         <v>4.8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="5">
         <v>21</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="8">
         <v>1.1000000000000001</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="5">
         <v>20</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5">
         <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="5">
         <v>2.7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="5">
         <v>6</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="5">
+      <c r="H8" s="6"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="15">
         <v>16</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="K8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="15">
         <v>4.13</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="5">
+      <c r="M8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="15">
         <v>21</v>
       </c>
-      <c r="O8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P8" s="7">
+      <c r="O8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="16">
         <v>44767</v>
       </c>
-      <c r="Q8" s="9"/>
+      <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="5">
         <v>2.14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="5">
         <v>7</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="5">
         <v>27</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -19714,53 +19735,58 @@
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5">
         <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5">
         <v>3.8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="5">
         <v>8</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="5">
+      <c r="H10" s="6"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="15">
         <v>6</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="K10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="17">
         <v>4.3</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="5">
+      <c r="M10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="15">
         <v>23</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="9"/>
+      <c r="O10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="16">
+        <v>44775</v>
+      </c>
+      <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5">
         <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -19768,88 +19794,95 @@
         <v>9</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="5">
         <v>9</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L11" s="5">
         <v>2.16</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N11" s="5">
         <v>24</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5">
         <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="5">
         <v>3.7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="5">
         <v>10</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="I12" s="9"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="5">
         <v>17</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L12" s="5">
         <v>4.16</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N12" s="5">
         <v>25</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="9"/>
+      <c r="Q12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="F13" s="15">
         <v>11</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="I13" s="9"/>
+      <c r="G13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="16">
+        <v>44769</v>
+      </c>
+      <c r="I13" s="13"/>
       <c r="J13" s="5">
         <v>25</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -19858,191 +19891,191 @@
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5">
+      <c r="A14" s="13"/>
+      <c r="B14" s="15">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="15">
         <v>4.18</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="15">
+        <v>12</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="16">
+        <v>44759</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15">
+        <v>2</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" s="15">
+        <v>1.22</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="15">
+        <v>27</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="16">
+        <v>44759</v>
+      </c>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="15">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="15">
+        <v>4.24</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="16">
+        <v>44759</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="15">
+        <v>4</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="15">
+        <v>28</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="16">
+        <v>44760</v>
+      </c>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="15">
+        <v>14</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="5">
-        <v>12</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="7">
+      <c r="D16" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="15">
+        <v>14</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="16">
+        <v>44764</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="15">
+        <v>8</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="15">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="15">
+        <v>29</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="16">
+        <v>44762</v>
+      </c>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="15">
+        <v>18</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="15">
+        <v>4.17</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="15">
+        <v>15</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="16">
         <v>44759</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="5">
-        <v>2</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="5">
-        <v>27</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P14" s="7">
-        <v>44759</v>
-      </c>
-      <c r="Q14" s="9"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="5">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="5">
-        <v>4.24</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="5">
-        <v>13</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="7">
-        <v>44759</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="5">
-        <v>4</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="5">
-        <v>28</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P15" s="7">
-        <v>44760</v>
-      </c>
-      <c r="Q15" s="9"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="5">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="5">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="7">
-        <v>44764</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="5">
-        <v>8</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="5">
-        <v>29</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="P16" s="7">
-        <v>44762</v>
-      </c>
-      <c r="Q16" s="9"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="5">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="5">
-        <v>15</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="7">
-        <v>44759</v>
-      </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="5">
         <v>20</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L17" s="5">
         <v>1.7</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N17" s="5">
         <v>30</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="9"/>
+      <c r="Q17" s="13"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>

</xml_diff>

<commit_message>
Finished writing the methods ...for now
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Documents\WCU\thesisschmesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4B91D3-D7B9-4B30-B73B-C6ACFA1C1EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090FC355-B3D6-4BA1-9F40-4A735FF79158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
@@ -222,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,8 +244,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +270,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -273,11 +285,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,9 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,9 +330,16 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8627,7 +8644,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="2">
-        <f>AVERAGE(O2:R2)</f>
+        <f t="shared" ref="N2:N33" si="0">AVERAGE(O2:R2)</f>
         <v>20.7</v>
       </c>
       <c r="O2" s="2">
@@ -8702,7 +8719,7 @@
         <v>17</v>
       </c>
       <c r="N3" s="2">
-        <f>AVERAGE(O3:R3)</f>
+        <f t="shared" si="0"/>
         <v>12.45</v>
       </c>
       <c r="O3" s="2">
@@ -8777,7 +8794,7 @@
         <v>17</v>
       </c>
       <c r="N4" s="2">
-        <f>AVERAGE(O4:R4)</f>
+        <f t="shared" si="0"/>
         <v>13.3</v>
       </c>
       <c r="O4" s="2">
@@ -8852,7 +8869,7 @@
         <v>17</v>
       </c>
       <c r="N5" s="2">
-        <f>AVERAGE(O5:R5)</f>
+        <f t="shared" si="0"/>
         <v>9.8749999999999982</v>
       </c>
       <c r="O5" s="2">
@@ -8918,7 +8935,7 @@
         <v>17</v>
       </c>
       <c r="N6" s="2">
-        <f>AVERAGE(O6:R6)</f>
+        <f t="shared" si="0"/>
         <v>8.8249999999999993</v>
       </c>
       <c r="O6" s="2">
@@ -8996,7 +9013,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="2">
-        <f>AVERAGE(O7:R7)</f>
+        <f t="shared" si="0"/>
         <v>13.024999999999999</v>
       </c>
       <c r="O7" s="2">
@@ -9074,7 +9091,7 @@
         <v>17</v>
       </c>
       <c r="N8" s="2">
-        <f>AVERAGE(O8:R8)</f>
+        <f t="shared" si="0"/>
         <v>13.15</v>
       </c>
       <c r="O8" s="2">
@@ -9146,7 +9163,7 @@
         <v>17</v>
       </c>
       <c r="N9" s="2">
-        <f>AVERAGE(O9:R9)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="O9" s="2">
@@ -9218,7 +9235,7 @@
         <v>17</v>
       </c>
       <c r="N10" s="2">
-        <f>AVERAGE(O10:R10)</f>
+        <f t="shared" si="0"/>
         <v>12.774999999999999</v>
       </c>
       <c r="O10" s="2">
@@ -9293,7 +9310,7 @@
         <v>17</v>
       </c>
       <c r="N11" s="2">
-        <f>AVERAGE(O11:R11)</f>
+        <f t="shared" si="0"/>
         <v>14.425000000000001</v>
       </c>
       <c r="O11" s="2">
@@ -9368,7 +9385,7 @@
         <v>17</v>
       </c>
       <c r="N12" s="2">
-        <f>AVERAGE(O12:R12)</f>
+        <f t="shared" si="0"/>
         <v>16.849999999999998</v>
       </c>
       <c r="O12" s="2">
@@ -9437,7 +9454,7 @@
         <v>17</v>
       </c>
       <c r="N13" s="2">
-        <f>AVERAGE(O13:R13)</f>
+        <f t="shared" si="0"/>
         <v>20.074999999999999</v>
       </c>
       <c r="O13" s="2">
@@ -9506,7 +9523,7 @@
         <v>17</v>
       </c>
       <c r="N14" s="2">
-        <f>AVERAGE(O14:R14)</f>
+        <f t="shared" si="0"/>
         <v>24.375</v>
       </c>
       <c r="O14" s="2">
@@ -9578,7 +9595,7 @@
         <v>17</v>
       </c>
       <c r="N15" s="2">
-        <f>AVERAGE(O15:R15)</f>
+        <f t="shared" si="0"/>
         <v>19.95</v>
       </c>
       <c r="O15" s="2">
@@ -9653,7 +9670,7 @@
         <v>17</v>
       </c>
       <c r="N16" s="2">
-        <f>AVERAGE(O16:R16)</f>
+        <f t="shared" si="0"/>
         <v>13.8</v>
       </c>
       <c r="O16" s="2">
@@ -9731,7 +9748,7 @@
         <v>17</v>
       </c>
       <c r="N17" s="2">
-        <f>AVERAGE(O17:R17)</f>
+        <f t="shared" si="0"/>
         <v>12.675000000000001</v>
       </c>
       <c r="O17" s="2">
@@ -9806,7 +9823,7 @@
         <v>17</v>
       </c>
       <c r="N18" s="2">
-        <f>AVERAGE(O18:R18)</f>
+        <f t="shared" si="0"/>
         <v>16.2</v>
       </c>
       <c r="O18" s="2">
@@ -9878,7 +9895,7 @@
         <v>17</v>
       </c>
       <c r="N19" s="2">
-        <f>AVERAGE(O19:R19)</f>
+        <f t="shared" si="0"/>
         <v>16.150000000000002</v>
       </c>
       <c r="O19" s="2">
@@ -9950,7 +9967,7 @@
         <v>17</v>
       </c>
       <c r="N20" s="2">
-        <f>AVERAGE(O20:R20)</f>
+        <f t="shared" si="0"/>
         <v>12.425000000000001</v>
       </c>
       <c r="O20" s="2">
@@ -10022,7 +10039,7 @@
         <v>17</v>
       </c>
       <c r="N21" s="2">
-        <f>AVERAGE(O21:R21)</f>
+        <f t="shared" si="0"/>
         <v>16.724999999999998</v>
       </c>
       <c r="O21" s="2">
@@ -10094,7 +10111,7 @@
         <v>17</v>
       </c>
       <c r="N22" s="2">
-        <f>AVERAGE(O22:R22)</f>
+        <f t="shared" si="0"/>
         <v>16.424999999999997</v>
       </c>
       <c r="O22" s="2">
@@ -10166,7 +10183,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="2">
-        <f>AVERAGE(O23:R23)</f>
+        <f t="shared" si="0"/>
         <v>12.725000000000001</v>
       </c>
       <c r="O23" s="2">
@@ -10238,7 +10255,7 @@
         <v>19</v>
       </c>
       <c r="N24" s="2">
-        <f>AVERAGE(O24:R24)</f>
+        <f t="shared" si="0"/>
         <v>12.25</v>
       </c>
       <c r="O24" s="2">
@@ -10307,7 +10324,7 @@
         <v>19</v>
       </c>
       <c r="N25" s="2">
-        <f>AVERAGE(O25:R25)</f>
+        <f t="shared" si="0"/>
         <v>10.6</v>
       </c>
       <c r="O25" s="2">
@@ -10376,7 +10393,7 @@
         <v>19</v>
       </c>
       <c r="N26" s="2">
-        <f>AVERAGE(O26:R26)</f>
+        <f t="shared" si="0"/>
         <v>16.125</v>
       </c>
       <c r="O26" s="2">
@@ -10445,7 +10462,7 @@
         <v>19</v>
       </c>
       <c r="N27" s="2">
-        <f>AVERAGE(O27:R27)</f>
+        <f t="shared" si="0"/>
         <v>8.3250000000000011</v>
       </c>
       <c r="O27" s="2">
@@ -10520,7 +10537,7 @@
         <v>19</v>
       </c>
       <c r="N28" s="2">
-        <f>AVERAGE(O28:R28)</f>
+        <f t="shared" si="0"/>
         <v>10.700000000000001</v>
       </c>
       <c r="O28" s="2">
@@ -10598,7 +10615,7 @@
         <v>17</v>
       </c>
       <c r="N29" s="2">
-        <f>AVERAGE(O29:R29)</f>
+        <f t="shared" si="0"/>
         <v>26.2</v>
       </c>
       <c r="O29" s="2">
@@ -10679,7 +10696,7 @@
         <v>17</v>
       </c>
       <c r="N30" s="2">
-        <f>AVERAGE(O30:R30)</f>
+        <f t="shared" si="0"/>
         <v>20.725000000000001</v>
       </c>
       <c r="O30" s="2">
@@ -10748,7 +10765,7 @@
         <v>17</v>
       </c>
       <c r="N31" s="2">
-        <f>AVERAGE(O31:R31)</f>
+        <f t="shared" si="0"/>
         <v>13.675000000000001</v>
       </c>
       <c r="O31" s="2">
@@ -10820,7 +10837,7 @@
         <v>17</v>
       </c>
       <c r="N32" s="2">
-        <f>AVERAGE(O32:R32)</f>
+        <f t="shared" si="0"/>
         <v>21.625</v>
       </c>
       <c r="O32" s="2">
@@ -10889,7 +10906,7 @@
         <v>17</v>
       </c>
       <c r="N33" s="2">
-        <f>AVERAGE(O33:R33)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="O33" s="2">
@@ -10961,7 +10978,7 @@
         <v>17</v>
       </c>
       <c r="N34" s="2">
-        <f>AVERAGE(O34:R34)</f>
+        <f t="shared" ref="N34:N65" si="1">AVERAGE(O34:R34)</f>
         <v>16.074999999999999</v>
       </c>
       <c r="O34" s="2">
@@ -11030,7 +11047,7 @@
         <v>17</v>
       </c>
       <c r="N35" s="2">
-        <f>AVERAGE(O35:R35)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="O35" s="2">
@@ -11102,7 +11119,7 @@
         <v>17</v>
       </c>
       <c r="N36" s="2">
-        <f>AVERAGE(O36:R36)</f>
+        <f t="shared" si="1"/>
         <v>10.25</v>
       </c>
       <c r="O36" s="2">
@@ -11177,7 +11194,7 @@
         <v>17</v>
       </c>
       <c r="N37" s="2">
-        <f>AVERAGE(O37:R37)</f>
+        <f t="shared" si="1"/>
         <v>10.225</v>
       </c>
       <c r="O37" s="2">
@@ -11249,7 +11266,7 @@
         <v>17</v>
       </c>
       <c r="N38" s="2">
-        <f>AVERAGE(O38:R38)</f>
+        <f t="shared" si="1"/>
         <v>15.4</v>
       </c>
       <c r="O38" s="2">
@@ -11321,7 +11338,7 @@
         <v>17</v>
       </c>
       <c r="N39" s="2">
-        <f>AVERAGE(O39:R39)</f>
+        <f t="shared" si="1"/>
         <v>10.85</v>
       </c>
       <c r="O39" s="2">
@@ -11393,7 +11410,7 @@
         <v>17</v>
       </c>
       <c r="N40" s="2">
-        <f>AVERAGE(O40:R40)</f>
+        <f t="shared" si="1"/>
         <v>12.8</v>
       </c>
       <c r="O40" s="2">
@@ -11468,7 +11485,7 @@
         <v>17</v>
       </c>
       <c r="N41" s="2">
-        <f>AVERAGE(O41:R41)</f>
+        <f t="shared" si="1"/>
         <v>12.924999999999999</v>
       </c>
       <c r="O41" s="2">
@@ -11537,7 +11554,7 @@
         <v>17</v>
       </c>
       <c r="N42" s="2">
-        <f>AVERAGE(O42:R42)</f>
+        <f t="shared" si="1"/>
         <v>15.975</v>
       </c>
       <c r="O42" s="2">
@@ -11615,7 +11632,7 @@
         <v>17</v>
       </c>
       <c r="N43" s="2">
-        <f>AVERAGE(O43:R43)</f>
+        <f t="shared" si="1"/>
         <v>11.75</v>
       </c>
       <c r="O43" s="2">
@@ -11687,7 +11704,7 @@
         <v>19</v>
       </c>
       <c r="N44" s="2">
-        <f>AVERAGE(O44:R44)</f>
+        <f t="shared" si="1"/>
         <v>18.675000000000001</v>
       </c>
       <c r="O44" s="2">
@@ -11756,7 +11773,7 @@
         <v>19</v>
       </c>
       <c r="N45" s="2">
-        <f>AVERAGE(O45:R45)</f>
+        <f t="shared" si="1"/>
         <v>16.3</v>
       </c>
       <c r="O45" s="2">
@@ -11825,7 +11842,7 @@
         <v>19</v>
       </c>
       <c r="N46" s="2">
-        <f>AVERAGE(O46:R46)</f>
+        <f t="shared" si="1"/>
         <v>15.274999999999999</v>
       </c>
       <c r="O46" s="2">
@@ -11915,7 +11932,7 @@
         <v>17</v>
       </c>
       <c r="N47" s="2">
-        <f>AVERAGE(O47:R47)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="O47" s="2">
@@ -11990,7 +12007,7 @@
         <v>17</v>
       </c>
       <c r="N48" s="2">
-        <f>AVERAGE(O48:R48)</f>
+        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
       <c r="O48" s="2">
@@ -12065,7 +12082,7 @@
         <v>17</v>
       </c>
       <c r="N49" s="2">
-        <f>AVERAGE(O49:R49)</f>
+        <f t="shared" si="1"/>
         <v>5.25</v>
       </c>
       <c r="O49" s="2">
@@ -12143,7 +12160,7 @@
         <v>17</v>
       </c>
       <c r="N50" s="2">
-        <f>AVERAGE(O50:R50)</f>
+        <f t="shared" si="1"/>
         <v>16.575000000000003</v>
       </c>
       <c r="O50" s="2">
@@ -12215,7 +12232,7 @@
         <v>17</v>
       </c>
       <c r="N51" s="2">
-        <f>AVERAGE(O51:R51)</f>
+        <f t="shared" si="1"/>
         <v>13.875</v>
       </c>
       <c r="O51" s="2">
@@ -12290,7 +12307,7 @@
         <v>17</v>
       </c>
       <c r="N52" s="2">
-        <f>AVERAGE(O52:R52)</f>
+        <f t="shared" si="1"/>
         <v>11.525</v>
       </c>
       <c r="O52" s="2">
@@ -12359,7 +12376,7 @@
         <v>17</v>
       </c>
       <c r="N53" s="2">
-        <f>AVERAGE(O53:R53)</f>
+        <f t="shared" si="1"/>
         <v>12.9</v>
       </c>
       <c r="O53" s="2">
@@ -12431,7 +12448,7 @@
         <v>17</v>
       </c>
       <c r="N54" s="2">
-        <f>AVERAGE(O54:R54)</f>
+        <f t="shared" si="1"/>
         <v>15.225</v>
       </c>
       <c r="O54" s="2">
@@ -12503,7 +12520,7 @@
         <v>17</v>
       </c>
       <c r="N55" s="2">
-        <f>AVERAGE(O55:R55)</f>
+        <f t="shared" si="1"/>
         <v>19.675000000000001</v>
       </c>
       <c r="O55" s="2">
@@ -12572,7 +12589,7 @@
         <v>17</v>
       </c>
       <c r="N56" s="2">
-        <f>AVERAGE(O56:R56)</f>
+        <f t="shared" si="1"/>
         <v>19.899999999999999</v>
       </c>
       <c r="O56" s="2">
@@ -12650,7 +12667,7 @@
         <v>17</v>
       </c>
       <c r="N57" s="2">
-        <f>AVERAGE(O57:R57)</f>
+        <f t="shared" si="1"/>
         <v>17.275000000000002</v>
       </c>
       <c r="O57" s="2">
@@ -12725,7 +12742,7 @@
         <v>17</v>
       </c>
       <c r="N58" s="2">
-        <f>AVERAGE(O58:R58)</f>
+        <f t="shared" si="1"/>
         <v>19.625</v>
       </c>
       <c r="O58" s="2">
@@ -12800,7 +12817,7 @@
         <v>17</v>
       </c>
       <c r="N59" s="2">
-        <f>AVERAGE(O59:R59)</f>
+        <f t="shared" si="1"/>
         <v>10.75</v>
       </c>
       <c r="O59" s="2">
@@ -12875,7 +12892,7 @@
         <v>17</v>
       </c>
       <c r="N60" s="2">
-        <f>AVERAGE(O60:R60)</f>
+        <f t="shared" si="1"/>
         <v>8.9499999999999993</v>
       </c>
       <c r="O60" s="2">
@@ -12953,7 +12970,7 @@
         <v>17</v>
       </c>
       <c r="N61" s="2">
-        <f>AVERAGE(O61:R61)</f>
+        <f t="shared" si="1"/>
         <v>20.524999999999999</v>
       </c>
       <c r="O61" s="2">
@@ -13028,7 +13045,7 @@
         <v>17</v>
       </c>
       <c r="N62" s="2">
-        <f>AVERAGE(O62:R62)</f>
+        <f t="shared" si="1"/>
         <v>19.45</v>
       </c>
       <c r="O62" s="2">
@@ -13094,7 +13111,7 @@
         <v>17</v>
       </c>
       <c r="N63" s="2">
-        <f>AVERAGE(O63:R63)</f>
+        <f t="shared" si="1"/>
         <v>13.524999999999999</v>
       </c>
       <c r="O63" s="2">
@@ -13163,7 +13180,7 @@
         <v>17</v>
       </c>
       <c r="N64" s="2">
-        <f>AVERAGE(O64:R64)</f>
+        <f t="shared" si="1"/>
         <v>13.375</v>
       </c>
       <c r="O64" s="2">
@@ -13235,7 +13252,7 @@
         <v>17</v>
       </c>
       <c r="N65" s="2">
-        <f>AVERAGE(O65:R65)</f>
+        <f t="shared" si="1"/>
         <v>14.399999999999999</v>
       </c>
       <c r="O65" s="2">
@@ -13304,7 +13321,7 @@
         <v>17</v>
       </c>
       <c r="N66" s="2">
-        <f>AVERAGE(O66:R66)</f>
+        <f t="shared" ref="N66:N97" si="2">AVERAGE(O66:R66)</f>
         <v>11.675000000000001</v>
       </c>
       <c r="O66" s="2">
@@ -13376,7 +13393,7 @@
         <v>17</v>
       </c>
       <c r="N67" s="2">
-        <f>AVERAGE(O67:R67)</f>
+        <f t="shared" si="2"/>
         <v>18.149999999999999</v>
       </c>
       <c r="O67" s="2">
@@ -13448,7 +13465,7 @@
         <v>17</v>
       </c>
       <c r="N68" s="2">
-        <f>AVERAGE(O68:R68)</f>
+        <f t="shared" si="2"/>
         <v>20.175000000000001</v>
       </c>
       <c r="O68" s="2">
@@ -13517,7 +13534,7 @@
         <v>19</v>
       </c>
       <c r="N69" s="2">
-        <f>AVERAGE(O69:R69)</f>
+        <f t="shared" si="2"/>
         <v>15.475</v>
       </c>
       <c r="O69" s="2">
@@ -13586,7 +13603,7 @@
         <v>19</v>
       </c>
       <c r="N70" s="2">
-        <f>AVERAGE(O70:R70)</f>
+        <f t="shared" si="2"/>
         <v>15.125</v>
       </c>
       <c r="O70" s="2">
@@ -13661,7 +13678,7 @@
         <v>19</v>
       </c>
       <c r="N71" s="2">
-        <f>AVERAGE(O71:R71)</f>
+        <f t="shared" si="2"/>
         <v>11.5</v>
       </c>
       <c r="O71" s="2">
@@ -13736,7 +13753,7 @@
         <v>19</v>
       </c>
       <c r="N72" s="2">
-        <f>AVERAGE(O72:R72)</f>
+        <f t="shared" si="2"/>
         <v>9.0749999999999993</v>
       </c>
       <c r="O72" s="2">
@@ -13808,7 +13825,7 @@
         <v>19</v>
       </c>
       <c r="N73" s="2">
-        <f>AVERAGE(O73:R73)</f>
+        <f t="shared" si="2"/>
         <v>15.05</v>
       </c>
       <c r="O73" s="2">
@@ -13883,7 +13900,7 @@
         <v>19</v>
       </c>
       <c r="N74" s="2">
-        <f>AVERAGE(O74:R74)</f>
+        <f t="shared" si="2"/>
         <v>17.049999999999997</v>
       </c>
       <c r="O74" s="2">
@@ -13958,7 +13975,7 @@
         <v>19</v>
       </c>
       <c r="N75" s="2">
-        <f>AVERAGE(O75:R75)</f>
+        <f t="shared" si="2"/>
         <v>13.674999999999999</v>
       </c>
       <c r="O75" s="2">
@@ -14027,7 +14044,7 @@
         <v>19</v>
       </c>
       <c r="N76" s="2">
-        <f>AVERAGE(O76:R76)</f>
+        <f t="shared" si="2"/>
         <v>14.700000000000001</v>
       </c>
       <c r="O76" s="2">
@@ -14096,7 +14113,7 @@
         <v>19</v>
       </c>
       <c r="N77" s="2">
-        <f>AVERAGE(O77:R77)</f>
+        <f t="shared" si="2"/>
         <v>17.625</v>
       </c>
       <c r="O77" s="2">
@@ -14174,7 +14191,7 @@
         <v>19</v>
       </c>
       <c r="N78" s="2">
-        <f>AVERAGE(O78:R78)</f>
+        <f t="shared" si="2"/>
         <v>11.575000000000001</v>
       </c>
       <c r="O78" s="2">
@@ -14249,7 +14266,7 @@
         <v>19</v>
       </c>
       <c r="N79" s="2">
-        <f>AVERAGE(O79:R79)</f>
+        <f t="shared" si="2"/>
         <v>15.175000000000001</v>
       </c>
       <c r="O79" s="2">
@@ -14327,7 +14344,7 @@
         <v>19</v>
       </c>
       <c r="N80" s="2">
-        <f>AVERAGE(O80:R80)</f>
+        <f t="shared" si="2"/>
         <v>12.025</v>
       </c>
       <c r="O80" s="2">
@@ -14396,7 +14413,7 @@
         <v>19</v>
       </c>
       <c r="N81" s="2">
-        <f>AVERAGE(O81:R81)</f>
+        <f t="shared" si="2"/>
         <v>5.6750000000000007</v>
       </c>
       <c r="O81" s="2">
@@ -14471,7 +14488,7 @@
         <v>19</v>
       </c>
       <c r="N82" s="2">
-        <f>AVERAGE(O82:R82)</f>
+        <f t="shared" si="2"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="O82" s="2">
@@ -14546,7 +14563,7 @@
         <v>19</v>
       </c>
       <c r="N83" s="2">
-        <f>AVERAGE(O83:R83)</f>
+        <f t="shared" si="2"/>
         <v>10.225</v>
       </c>
       <c r="O83" s="2">
@@ -14624,7 +14641,7 @@
         <v>19</v>
       </c>
       <c r="N84" s="2">
-        <f>AVERAGE(O84:R84)</f>
+        <f t="shared" si="2"/>
         <v>13.899999999999999</v>
       </c>
       <c r="O84" s="2">
@@ -14702,7 +14719,7 @@
         <v>19</v>
       </c>
       <c r="N85" s="2">
-        <f>AVERAGE(O85:R85)</f>
+        <f t="shared" si="2"/>
         <v>11.1</v>
       </c>
       <c r="O85" s="2">
@@ -14783,7 +14800,7 @@
         <v>19</v>
       </c>
       <c r="N86" s="2">
-        <f>AVERAGE(O86:R86)</f>
+        <f t="shared" si="2"/>
         <v>8.0250000000000004</v>
       </c>
       <c r="O86" s="2">
@@ -14852,7 +14869,7 @@
         <v>19</v>
       </c>
       <c r="N87" s="2">
-        <f>AVERAGE(O87:R87)</f>
+        <f t="shared" si="2"/>
         <v>12.9</v>
       </c>
       <c r="O87" s="2">
@@ -14936,7 +14953,7 @@
         <v>17</v>
       </c>
       <c r="N88" s="2">
-        <f>AVERAGE(O88:R88)</f>
+        <f t="shared" si="2"/>
         <v>11.074999999999999</v>
       </c>
       <c r="O88" s="2">
@@ -15008,7 +15025,7 @@
         <v>17</v>
       </c>
       <c r="N89" s="2">
-        <f>AVERAGE(O89:R89)</f>
+        <f t="shared" si="2"/>
         <v>13.65</v>
       </c>
       <c r="O89" s="2">
@@ -15080,7 +15097,7 @@
         <v>17</v>
       </c>
       <c r="N90" s="2">
-        <f>AVERAGE(O90:R90)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O90" s="2">
@@ -15155,7 +15172,7 @@
         <v>17</v>
       </c>
       <c r="N91" s="2">
-        <f>AVERAGE(O91:R91)</f>
+        <f t="shared" si="2"/>
         <v>18.350000000000001</v>
       </c>
       <c r="O91" s="2">
@@ -15230,7 +15247,7 @@
         <v>17</v>
       </c>
       <c r="N92" s="2">
-        <f>AVERAGE(O92:R92)</f>
+        <f t="shared" si="2"/>
         <v>19.125</v>
       </c>
       <c r="O92" s="2">
@@ -15302,7 +15319,7 @@
         <v>17</v>
       </c>
       <c r="N93" s="2">
-        <f>AVERAGE(O93:R93)</f>
+        <f t="shared" si="2"/>
         <v>14.425000000000001</v>
       </c>
       <c r="O93" s="2">
@@ -15380,7 +15397,7 @@
         <v>17</v>
       </c>
       <c r="N94" s="2">
-        <f>AVERAGE(O94:R94)</f>
+        <f t="shared" si="2"/>
         <v>14.850000000000001</v>
       </c>
       <c r="O94" s="2">
@@ -15449,7 +15466,7 @@
         <v>17</v>
       </c>
       <c r="N95" s="2">
-        <f>AVERAGE(O95:R95)</f>
+        <f t="shared" si="2"/>
         <v>16.850000000000001</v>
       </c>
       <c r="O95" s="2">
@@ -15524,7 +15541,7 @@
         <v>17</v>
       </c>
       <c r="N96" s="2">
-        <f>AVERAGE(O96:R96)</f>
+        <f t="shared" si="2"/>
         <v>11.125</v>
       </c>
       <c r="O96" s="2">
@@ -15599,7 +15616,7 @@
         <v>17</v>
       </c>
       <c r="N97" s="2">
-        <f>AVERAGE(O97:R97)</f>
+        <f t="shared" si="2"/>
         <v>11.15</v>
       </c>
       <c r="O97" s="2">
@@ -15680,7 +15697,7 @@
         <v>17</v>
       </c>
       <c r="N98" s="2">
-        <f>AVERAGE(O98:R98)</f>
+        <f t="shared" ref="N98:N129" si="3">AVERAGE(O98:R98)</f>
         <v>16.600000000000001</v>
       </c>
       <c r="O98" s="2">
@@ -15749,7 +15766,7 @@
         <v>17</v>
       </c>
       <c r="N99" s="2">
-        <f>AVERAGE(O99:R99)</f>
+        <f t="shared" si="3"/>
         <v>9.7000000000000011</v>
       </c>
       <c r="O99" s="2">
@@ -15821,7 +15838,7 @@
         <v>17</v>
       </c>
       <c r="N100" s="2">
-        <f>AVERAGE(O100:R100)</f>
+        <f t="shared" si="3"/>
         <v>14.274999999999999</v>
       </c>
       <c r="O100" s="2">
@@ -19390,7 +19407,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19401,25 +19418,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -19488,25 +19505,25 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="15">
+      <c r="J3" s="14">
         <v>1</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="14">
         <v>1.21</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>16</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <v>44767</v>
       </c>
       <c r="Q3" s="13"/>
@@ -19531,58 +19548,58 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <v>7</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="14">
         <v>1.1299999999999999</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <v>17</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <v>44767</v>
       </c>
       <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="5">
+      <c r="B5" s="18">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18">
         <v>3</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="5">
+      <c r="J5" s="18">
         <v>30</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5">
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18">
         <v>18</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -19605,19 +19622,19 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="5">
+      <c r="J6" s="18">
         <v>26</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5">
-        <v>19</v>
-      </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18">
+        <v>19</v>
+      </c>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
       <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -19679,25 +19696,25 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <v>16</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="14">
         <v>4.13</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="14">
         <v>21</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <v>44767</v>
       </c>
       <c r="Q8" s="13"/>
@@ -19722,19 +19739,19 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="5">
+      <c r="J9" s="18">
         <v>27</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5">
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18">
         <v>22</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -19757,44 +19774,44 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <v>6</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>4.3</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="14">
         <v>23</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="15">
         <v>44775</v>
       </c>
       <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="5">
+      <c r="B11" s="18">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18">
         <v>9</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="13"/>
       <c r="J11" s="5">
         <v>9</v>
@@ -19856,205 +19873,205 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>11</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>3.1</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>11</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <v>44769</v>
       </c>
       <c r="I13" s="13"/>
-      <c r="J13" s="5">
+      <c r="J13" s="18">
         <v>25</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5">
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18">
         <v>26</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
       <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>24</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>4.18</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>12</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <v>44759</v>
       </c>
       <c r="I14" s="13"/>
-      <c r="J14" s="15">
+      <c r="J14" s="14">
         <v>2</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="14">
         <v>1.22</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="14">
         <v>27</v>
       </c>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="15">
         <v>44759</v>
       </c>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>4.24</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>13</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>44759</v>
       </c>
       <c r="I15" s="13"/>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <v>4</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="14">
         <v>28</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="15">
         <v>44760</v>
       </c>
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>14</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>2.8</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>14</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <v>44764</v>
       </c>
       <c r="I16" s="13"/>
-      <c r="J16" s="15">
+      <c r="J16" s="14">
         <v>8</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="14">
         <v>1.1599999999999999</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="14">
         <v>29</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="15">
         <v>44762</v>
       </c>
       <c r="Q16" s="13"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>18</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>4.17</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>15</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <v>44759</v>
       </c>
       <c r="I17" s="13"/>

</xml_diff>

<commit_message>
Re-did the arcGIS maps Tried to do RCBD on soil growth
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Documents\WCU\thesisschmesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Desktop\WCU\thesisschmesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090FC355-B3D6-4BA1-9F40-4A735FF79158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8899A8-163E-44BA-8DD7-BEF87D5BB61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="58">
   <si>
     <t>Transect</t>
   </si>
@@ -208,10 +208,10 @@
     <t>Current Order</t>
   </si>
   <si>
-    <t>Random #1</t>
+    <t>n</t>
   </si>
   <si>
-    <t>Random #2</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -330,10 +330,10 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -15697,7 +15697,7 @@
         <v>17</v>
       </c>
       <c r="N98" s="2">
-        <f t="shared" ref="N98:N129" si="3">AVERAGE(O98:R98)</f>
+        <f t="shared" ref="N98:N100" si="3">AVERAGE(O98:R98)</f>
         <v>16.600000000000001</v>
       </c>
       <c r="O98" s="2">
@@ -18675,7 +18675,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18700,7 +18700,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>53</v>
@@ -18708,15 +18708,9 @@
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -18734,7 +18728,9 @@
       <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
@@ -18756,7 +18752,9 @@
       <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
@@ -18774,7 +18772,9 @@
       <c r="D4" s="5">
         <v>3</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
@@ -18796,7 +18796,9 @@
       <c r="D5" s="5">
         <v>4</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
@@ -18818,7 +18820,9 @@
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
@@ -18840,7 +18844,9 @@
       <c r="D7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6"/>
@@ -18862,7 +18868,9 @@
       <c r="D8" s="5">
         <v>7</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
       <c r="H8" s="6"/>
@@ -18884,7 +18892,9 @@
       <c r="D9" s="5">
         <v>8</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="5"/>
       <c r="H9" s="6"/>
@@ -18902,7 +18912,9 @@
       <c r="D10" s="5">
         <v>9</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
@@ -18924,7 +18936,9 @@
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
@@ -18937,7 +18951,7 @@
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="8">
         <v>3.1</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -18946,8 +18960,12 @@
       <c r="D12" s="5">
         <v>11</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44769</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -18969,7 +18987,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F13" s="7">
         <v>44759</v>
@@ -18995,7 +19013,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F14" s="7">
         <v>44759</v>
@@ -19021,7 +19039,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F15" s="7">
         <v>44764</v>
@@ -19047,7 +19065,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F16" s="7">
         <v>44759</v>
@@ -19073,7 +19091,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F17" s="7">
         <v>44767</v>
@@ -19099,7 +19117,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F18" s="7">
         <v>44767</v>
@@ -19120,7 +19138,9 @@
       <c r="D19" s="5">
         <v>18</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="5"/>
       <c r="H19" s="6"/>
@@ -19138,7 +19158,9 @@
       <c r="D20" s="5">
         <v>19</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
@@ -19160,7 +19182,9 @@
       <c r="D21" s="5">
         <v>20</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
@@ -19183,7 +19207,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F22" s="7">
         <v>44767</v>
@@ -19204,7 +19228,9 @@
       <c r="D23" s="5">
         <v>22</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
@@ -19217,7 +19243,7 @@
       <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="8">
         <v>4.3</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -19226,8 +19252,12 @@
       <c r="D24" s="5">
         <v>23</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="7">
+        <v>44775</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -19248,7 +19278,9 @@
       <c r="D25" s="5">
         <v>24</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
       <c r="H25" s="6"/>
@@ -19270,7 +19302,9 @@
       <c r="D26" s="5">
         <v>25</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
       <c r="H26" s="6"/>
@@ -19288,7 +19322,9 @@
       <c r="D27" s="5">
         <v>26</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5"/>
       <c r="H27" s="6"/>
@@ -19311,7 +19347,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F28" s="7">
         <v>44759</v>
@@ -19337,7 +19373,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F29" s="7">
         <v>44760</v>
@@ -19363,7 +19399,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F30" s="7">
         <v>44762</v>
@@ -19388,7 +19424,9 @@
       <c r="D31" s="5">
         <v>30</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="5"/>
       <c r="H31" s="6"/>
@@ -19418,25 +19456,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -19573,33 +19611,33 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>28</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17">
         <v>3</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <v>30</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18">
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17">
         <v>18</v>
       </c>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
       <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -19622,19 +19660,19 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>26</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18">
-        <v>19</v>
-      </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17">
+        <v>19</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
       <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -19739,19 +19777,19 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <v>27</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17">
         <v>22</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -19799,19 +19837,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>29</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17">
         <v>9</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="13"/>
       <c r="J11" s="5">
         <v>9</v>
@@ -19895,19 +19933,19 @@
         <v>44769</v>
       </c>
       <c r="I13" s="13"/>
-      <c r="J13" s="18">
+      <c r="J13" s="17">
         <v>25</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18">
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17">
         <v>26</v>
       </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tried out some code after updating for the longest effin time
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Desktop\WCU\thesisschmesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8899A8-163E-44BA-8DD7-BEF87D5BB61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F82D38-19ED-4D79-AC06-811D51DBEB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
     <sheet name="Ground Cover" sheetId="2" r:id="rId2"/>
-    <sheet name="Soil Samples" sheetId="3" r:id="rId3"/>
-    <sheet name="Random" sheetId="4" r:id="rId4"/>
+    <sheet name="Soil Samples (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="Soil Samples" sheetId="3" r:id="rId4"/>
+    <sheet name="Random" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="58">
   <si>
     <t>Transect</t>
   </si>
@@ -222,7 +223,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +248,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,12 +293,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -333,14 +342,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -18671,11 +18684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5379496-B6C4-421B-9D7D-11C06426F583}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19F489C-E848-4FB5-B46A-8E1D9FCFE178}">
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18717,16 +18730,12 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="5">
-        <v>3.23</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>56</v>
@@ -18741,16 +18750,12 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>56</v>
@@ -18770,7 +18775,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>56</v>
@@ -18785,16 +18790,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="5">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>56</v>
@@ -18809,16 +18810,12 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="5">
-        <v>4.8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="5">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>56</v>
@@ -18833,16 +18830,12 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="5">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>56</v>
@@ -18860,13 +18853,13 @@
         <v>48</v>
       </c>
       <c r="B8" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>3.23</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.25</v>
       </c>
       <c r="D8" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>56</v>
@@ -18886,8 +18879,8 @@
       <c r="B9" s="5">
         <v>3.8</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>49</v>
+      <c r="C9" s="18">
+        <v>0.25</v>
       </c>
       <c r="D9" s="5">
         <v>8</v>
@@ -18905,15 +18898,792 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="5">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44769</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44767</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="C12" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="5">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="5">
+        <v>29</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44762</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2.14</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>7</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4.24</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="5">
+        <v>13</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44759</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>16</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44767</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="C17" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>23</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="7">
+        <v>44775</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1.22</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="7">
+        <v>44759</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44760</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D22" s="5">
+        <v>10</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4.18</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="5">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="7">
+        <v>44759</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="5">
+        <v>20</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="5">
+        <v>30</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="C28" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="5">
+        <v>14</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="7">
+        <v>44764</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4.17</v>
+      </c>
+      <c r="C29" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="5">
+        <v>15</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="7">
+        <v>44759</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4.13</v>
+      </c>
+      <c r="C30" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="5">
+        <v>21</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="7">
+        <v>44767</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="C31" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="5">
+        <v>25</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
+    <sortCondition ref="A1:A31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5379496-B6C4-421B-9D7D-11C06426F583}">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3.23</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.25</v>
+      </c>
       <c r="D10" s="5">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
@@ -18925,19 +19695,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
+        <v>2.14</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.5</v>
       </c>
       <c r="D11" s="5">
-        <v>10</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
@@ -18954,14 +19724,14 @@
       <c r="B12" s="8">
         <v>3.1</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>49</v>
+      <c r="C12" s="18">
+        <v>0.25</v>
       </c>
       <c r="D12" s="5">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>57</v>
+      <c r="E12" s="6">
+        <v>1</v>
       </c>
       <c r="F12" s="7">
         <v>44769</v>
@@ -18975,22 +19745,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5">
-        <v>4.18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>49</v>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.25</v>
       </c>
       <c r="D13" s="5">
-        <v>12</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
       </c>
       <c r="F13" s="7">
-        <v>44759</v>
+        <v>44767</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
@@ -19004,19 +19774,19 @@
         <v>48</v>
       </c>
       <c r="B14" s="5">
-        <v>4.24</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>52</v>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.25</v>
       </c>
       <c r="D14" s="5">
-        <v>13</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
       </c>
       <c r="F14" s="7">
-        <v>44759</v>
+        <v>44762</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
@@ -19027,22 +19797,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>4.24</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.5</v>
       </c>
       <c r="D15" s="5">
-        <v>14</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>57</v>
+        <v>13</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
       </c>
       <c r="F15" s="7">
-        <v>44764</v>
+        <v>44759</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="6"/>
@@ -19053,22 +19823,22 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>52</v>
+        <v>1.21</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0.5</v>
       </c>
       <c r="D16" s="5">
-        <v>15</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
       </c>
       <c r="F16" s="7">
-        <v>44759</v>
+        <v>44767</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="6"/>
@@ -19081,20 +19851,20 @@
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="5">
-        <v>1.21</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>52</v>
+      <c r="B17" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="C17" s="18">
+        <v>0.5</v>
       </c>
       <c r="D17" s="5">
-        <v>16</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>57</v>
+        <v>23</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>44767</v>
+        <v>44775</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="6"/>
@@ -19108,19 +19878,19 @@
         <v>48</v>
       </c>
       <c r="B18" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>1.22</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.5</v>
       </c>
       <c r="D18" s="5">
-        <v>17</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>57</v>
+        <v>27</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
       </c>
       <c r="F18" s="7">
-        <v>44767</v>
+        <v>44759</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
@@ -19131,17 +19901,23 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0.5</v>
+      </c>
       <c r="D19" s="5">
-        <v>18</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44760</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -19151,15 +19927,19 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B20" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.25</v>
+      </c>
       <c r="D20" s="5">
-        <v>19</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>56</v>
+        <v>2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="5"/>
@@ -19173,17 +19953,17 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>49</v>
+      <c r="B21" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.25</v>
       </c>
       <c r="D21" s="5">
-        <v>20</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
@@ -19198,20 +19978,18 @@
         <v>50</v>
       </c>
       <c r="B22" s="5">
-        <v>4.13</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>3.7</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0.25</v>
       </c>
       <c r="D22" s="5">
-        <v>21</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="7">
-        <v>44767</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="5"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -19221,15 +19999,19 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0.25</v>
+      </c>
       <c r="D23" s="5">
-        <v>22</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>56</v>
+        <v>20</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="5"/>
@@ -19241,23 +20023,21 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.25</v>
       </c>
       <c r="D24" s="5">
-        <v>23</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="7">
-        <v>44775</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6"/>
       <c r="G24" s="5"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -19267,19 +20047,19 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5">
-        <v>2.16</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>49</v>
+        <v>4.8</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0.5</v>
       </c>
       <c r="D25" s="5">
-        <v>24</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
@@ -19294,16 +20074,16 @@
         <v>50</v>
       </c>
       <c r="B26" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>52</v>
+        <v>2.7</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.5</v>
       </c>
       <c r="D26" s="5">
-        <v>25</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
@@ -19315,15 +20095,19 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B27" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0.5</v>
+      </c>
       <c r="D27" s="5">
-        <v>26</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>56</v>
+        <v>25</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5"/>
@@ -19335,19 +20119,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>4.18</v>
+      </c>
+      <c r="C28" s="18">
+        <v>0.25</v>
       </c>
       <c r="D28" s="5">
-        <v>27</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>57</v>
+        <v>12</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
       </c>
       <c r="F28" s="7">
         <v>44759</v>
@@ -19361,22 +20145,22 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="C29" s="18">
+        <v>0.5</v>
       </c>
       <c r="D29" s="5">
-        <v>28</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>57</v>
+        <v>14</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1</v>
       </c>
       <c r="F29" s="7">
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="6"/>
@@ -19387,22 +20171,22 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>49</v>
+        <v>4.17</v>
+      </c>
+      <c r="C30" s="18">
+        <v>0.5</v>
       </c>
       <c r="D30" s="5">
-        <v>29</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1</v>
       </c>
       <c r="F30" s="7">
-        <v>44762</v>
+        <v>44759</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>
@@ -19416,18 +20200,20 @@
         <v>50</v>
       </c>
       <c r="B31" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>4.13</v>
+      </c>
+      <c r="C31" s="18">
+        <v>0.5</v>
       </c>
       <c r="D31" s="5">
-        <v>30</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>44767</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -19436,15 +20222,18 @@
       <c r="L31" s="6"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
+    <sortCondition ref="A1:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70826AB2-0F3B-43B6-8E74-FD8F1FFA7EF4}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -19456,25 +20245,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>

</xml_diff>

<commit_message>
randomized soil samples in data sheet
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Desktop\WCU\thesisschmesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F82D38-19ED-4D79-AC06-811D51DBEB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE8E65E-B043-4B75-B0B7-98822B8DA9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
+    <workbookView xWindow="-2370" yWindow="5985" windowWidth="11565" windowHeight="8865" activeTab="2" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
     <sheet name="Ground Cover" sheetId="2" r:id="rId2"/>
-    <sheet name="Soil Samples (2)" sheetId="5" r:id="rId3"/>
-    <sheet name="Soil Samples" sheetId="3" r:id="rId4"/>
-    <sheet name="Random" sheetId="4" r:id="rId5"/>
+    <sheet name="Soil Samples" sheetId="3" r:id="rId3"/>
+    <sheet name="Random" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="58">
   <si>
     <t>Transect</t>
   </si>
@@ -209,10 +208,10 @@
     <t>Current Order</t>
   </si>
   <si>
-    <t>n</t>
+    <t>y</t>
   </si>
   <si>
-    <t>y</t>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -15901,8 +15900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA563366-8DA0-4A43-8949-852B034D9918}">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -18684,1563 +18683,847 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19F489C-E848-4FB5-B46A-8E1D9FCFE178}">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5379496-B6C4-421B-9D7D-11C06426F583}">
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="5">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4.13</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="7">
+        <v>44767</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4.24</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="G6" s="7">
+        <v>44759</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3.23</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="7">
+        <v>44760</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="7">
+        <v>44775</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="5">
+        <v>12</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="7">
+        <v>44764</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="5">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="7">
+        <v>44762</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>14</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>29</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <v>15</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>27</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5">
+        <v>16</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>21</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="5">
+        <v>17</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D19" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="5">
+        <v>18</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7">
+        <v>44767</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="D20" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="5">
+        <v>19</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="7">
+        <v>44769</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4.17</v>
+      </c>
+      <c r="D22" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="5">
+        <v>21</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="7">
+        <v>44759</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1.22</v>
+      </c>
+      <c r="D23" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="5">
+        <v>22</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="7">
+        <v>44759</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="D24" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E24" s="5">
+        <v>23</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>13</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="D25" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="5">
+        <v>24</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E26" s="5">
+        <v>25</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>20</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="D27" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="5">
+        <v>26</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2.14</v>
+      </c>
+      <c r="D28" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="5">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="D29" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="5">
+        <v>28</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="G29" s="7">
+        <v>44767</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>24</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="5">
+        <v>4.18</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="5">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="7">
+        <v>44759</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5">
-        <v>3.23</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="5">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="8">
-        <v>3.1</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D10" s="5">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="7">
-        <v>44769</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="C11" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D11" s="5">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2.16</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D12" s="5">
-        <v>24</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D13" s="5">
-        <v>29</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44762</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="C14" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>7</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5">
-        <v>4.24</v>
-      </c>
-      <c r="C15" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1.21</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>23</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="7">
-        <v>44775</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="5">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="5">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="7">
-        <v>44760</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="5">
-        <v>4</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D22" s="5">
-        <v>10</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="5">
-        <v>4.18</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D23" s="5">
-        <v>12</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D24" s="5">
-        <v>20</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D25" s="5">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5">
         <v>30</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="5">
-        <v>4.8</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>5</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="5">
-        <v>6</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D28" s="5">
-        <v>14</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="7">
-        <v>44764</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="C29" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D29" s="5">
-        <v>15</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5">
-        <v>4.13</v>
-      </c>
-      <c r="C30" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="5">
-        <v>21</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="C31" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D31" s="5">
-        <v>25</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="F31" s="6"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="5"/>
       <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
-    <sortCondition ref="A1:A31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
+    <sortCondition ref="E1:E31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5379496-B6C4-421B-9D7D-11C06426F583}">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70826AB2-0F3B-43B6-8E74-FD8F1FFA7EF4}">
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5">
-        <v>3.23</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="5">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2.16</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D10" s="5">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="C11" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="5">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="8">
-        <v>3.1</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D12" s="5">
-        <v>11</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>44769</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D13" s="5">
-        <v>17</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C14" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D14" s="5">
-        <v>29</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>44762</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5">
-        <v>4.24</v>
-      </c>
-      <c r="C15" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1.21</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>23</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7">
-        <v>44775</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="5">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="5">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7">
-        <v>44760</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="5">
-        <v>4</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D22" s="5">
-        <v>10</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D23" s="5">
-        <v>20</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D24" s="5">
-        <v>30</v>
-      </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="5">
-        <v>4.8</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D25" s="5">
-        <v>5</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>6</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="5">
-        <v>25</v>
-      </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5">
-        <v>4.18</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="D28" s="5">
-        <v>12</v>
-      </c>
-      <c r="E28" s="6">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="C29" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D29" s="5">
-        <v>14</v>
-      </c>
-      <c r="E29" s="6">
-        <v>1</v>
-      </c>
-      <c r="F29" s="7">
-        <v>44764</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="C30" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="5">
-        <v>15</v>
-      </c>
-      <c r="E30" s="6">
-        <v>1</v>
-      </c>
-      <c r="F30" s="7">
-        <v>44759</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="5">
-        <v>4.13</v>
-      </c>
-      <c r="C31" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="D31" s="5">
-        <v>21</v>
-      </c>
-      <c r="E31" s="6">
-        <v>1</v>
-      </c>
-      <c r="F31" s="7">
-        <v>44767</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
-    <sortCondition ref="A1:A32"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70826AB2-0F3B-43B6-8E74-FD8F1FFA7EF4}">
-  <dimension ref="A1:Q32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20314,189 +19597,205 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="5">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3.23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="B3" s="17">
+        <v>30</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17">
         <v>1</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="14">
-        <v>1</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="14">
-        <v>1.21</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="14">
+      <c r="J3" s="17">
+        <v>27</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17">
         <v>16</v>
       </c>
-      <c r="O3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="15">
-        <v>44767</v>
-      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
       <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="5">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="14">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="15">
+        <v>44767</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="5">
+        <v>21</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="5">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14">
-        <v>7</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="14">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" s="14">
+      <c r="N4" s="6">
         <v>17</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="15">
-        <v>44767</v>
-      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
       <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="17">
-        <v>28</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17">
+      <c r="B5" s="5">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="17">
-        <v>30</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17">
+      <c r="J5" s="14">
+        <v>7</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="14">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="14">
         <v>18</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" s="15">
+        <v>44767</v>
+      </c>
       <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="5">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="B6" s="14">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="14">
         <v>4</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="15">
+        <v>44785</v>
+      </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="17">
-        <v>26</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17">
-        <v>19</v>
-      </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="J6" s="14">
+        <v>11</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="14">
+        <v>19</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="15">
+        <v>44769</v>
+      </c>
       <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="5">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="5">
-        <v>4.8</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="14">
+        <v>4.24</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="15">
+        <v>44759</v>
+      </c>
       <c r="I7" s="13"/>
       <c r="J7" s="5">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="8">
-        <v>1.1000000000000001</v>
+      <c r="L7" s="5">
+        <v>4.16</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="5">
+        <v>52</v>
+      </c>
+      <c r="N7" s="6">
         <v>20</v>
       </c>
       <c r="O7" s="6"/>
@@ -20506,31 +19805,31 @@
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="5">
-        <v>2.7</v>
+        <v>3.23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="5">
+        <v>49</v>
+      </c>
+      <c r="F8" s="6">
         <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="13"/>
       <c r="J8" s="14">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>50</v>
       </c>
       <c r="L8" s="14">
-        <v>4.13</v>
+        <v>4.17</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>52</v>
@@ -20542,76 +19841,88 @@
         <v>54</v>
       </c>
       <c r="P8" s="15">
-        <v>44767</v>
+        <v>44759</v>
       </c>
       <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="5">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="14">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="14">
         <v>7</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="15">
+        <v>44760</v>
+      </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="17">
-        <v>27</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17">
+      <c r="J9" s="14">
+        <v>2</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="14">
+        <v>1.22</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="14">
         <v>22</v>
       </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
+      <c r="O9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="15">
+        <v>44759</v>
+      </c>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="5">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="5">
+        <v>52</v>
+      </c>
+      <c r="F10" s="6">
         <v>8</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="13"/>
       <c r="J10" s="14">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="16">
-        <v>4.3</v>
+      <c r="L10" s="14">
+        <v>2.16</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N10" s="14">
         <v>23</v>
@@ -20620,39 +19931,43 @@
         <v>54</v>
       </c>
       <c r="P10" s="15">
-        <v>44775</v>
+        <v>44783</v>
       </c>
       <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="17">
-        <v>29</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17">
+      <c r="B11" s="5">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="6">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="13"/>
       <c r="J11" s="5">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L11" s="5">
-        <v>2.16</v>
+        <v>2.7</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" s="5">
+        <v>52</v>
+      </c>
+      <c r="N11" s="6">
         <v>24</v>
       </c>
       <c r="O11" s="6"/>
@@ -20661,95 +19976,99 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
-      <c r="B12" s="5">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="14">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="16">
+        <v>4.3</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="14">
+        <v>10</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="15">
+        <v>44775</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14">
+        <v>22</v>
+      </c>
+      <c r="K12" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="L12" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="M12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="5">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="5">
-        <v>17</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="5">
+      <c r="N12" s="14">
         <v>25</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="O12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="15">
+        <v>44783</v>
+      </c>
       <c r="Q12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="14">
+      <c r="B13" s="17">
+        <v>28</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17">
         <v>11</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="16">
-        <v>3.1</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="5">
+        <v>20</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="14">
-        <v>11</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="15">
-        <v>44769</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="17">
-        <v>25</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17">
+      <c r="N13" s="6">
         <v>26</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="14">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="14">
-        <v>4.18</v>
+        <v>2.8</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F14" s="14">
         <v>12</v>
@@ -20758,17 +20077,17 @@
         <v>54</v>
       </c>
       <c r="H14" s="15">
-        <v>44759</v>
+        <v>44764</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>48</v>
       </c>
       <c r="L14" s="14">
-        <v>1.22</v>
+        <v>2.14</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>52</v>
@@ -20780,23 +20099,23 @@
         <v>54</v>
       </c>
       <c r="P14" s="15">
-        <v>44759</v>
+        <v>44783</v>
       </c>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="14">
-        <v>4.24</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="14">
         <v>13</v>
@@ -20805,17 +20124,17 @@
         <v>54</v>
       </c>
       <c r="H15" s="15">
-        <v>44759</v>
+        <v>44762</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="16">
-        <v>2.2000000000000002</v>
+      <c r="L15" s="14">
+        <v>1.21</v>
       </c>
       <c r="M15" s="14" t="s">
         <v>52</v>
@@ -20827,42 +20146,34 @@
         <v>54</v>
       </c>
       <c r="P15" s="15">
-        <v>44760</v>
+        <v>44767</v>
       </c>
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="14">
+      <c r="B16" s="17">
+        <v>25</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17">
         <v>14</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="14">
-        <v>2.8</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="14">
-        <v>14</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="15">
-        <v>44764</v>
-      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="13"/>
       <c r="J16" s="14">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L16" s="14">
-        <v>1.1599999999999999</v>
+        <v>4.18</v>
       </c>
       <c r="M16" s="14" t="s">
         <v>49</v>
@@ -20874,51 +20185,39 @@
         <v>54</v>
       </c>
       <c r="P16" s="15">
-        <v>44762</v>
+        <v>44759</v>
       </c>
       <c r="Q16" s="13"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="14">
-        <v>18</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="14">
-        <v>4.17</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="14">
+      <c r="B17" s="17">
+        <v>29</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17">
         <v>15</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="15">
-        <v>44759</v>
-      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="5">
-        <v>20</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N17" s="5">
+      <c r="J17" s="17">
+        <v>26</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17">
         <v>30</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -20940,133 +20239,10 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B20:H49">
+    <sortCondition ref="F20:F49"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>

</xml_diff>

<commit_message>
apparantlee some gis changes I also randomized this months soils samples
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd791bf81ccb4a31/Desktop/WCU/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonhi\OneDrive\Desktop\WCU\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{5BE8E65E-B043-4B75-B0B7-98822B8DA9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3E83A8-11C0-4DD0-A355-00D19330E3BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC0CD11-A4AE-48F4-AC91-9FCB5EA3DC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="57">
   <si>
     <t>Transect</t>
   </si>
@@ -192,6 +192,24 @@
   <si>
     <t>Original</t>
   </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -264,6 +282,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,38 +611,38 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -719,7 +743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>6</v>
       </c>
@@ -794,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -869,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>6</v>
       </c>
@@ -944,7 +968,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>6</v>
       </c>
@@ -1010,7 +1034,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>6</v>
       </c>
@@ -1088,7 +1112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1166,7 +1190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1238,7 +1262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -1310,7 +1334,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -1385,7 +1409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -1460,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1529,7 +1553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -1598,7 +1622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>6</v>
       </c>
@@ -1670,7 +1694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>6</v>
       </c>
@@ -1745,7 +1769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>6</v>
       </c>
@@ -1823,7 +1847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>6</v>
       </c>
@@ -1898,7 +1922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>6</v>
       </c>
@@ -1970,7 +1994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>6</v>
       </c>
@@ -2042,7 +2066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>6</v>
       </c>
@@ -2114,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>6</v>
       </c>
@@ -2186,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>6</v>
       </c>
@@ -2258,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>6</v>
       </c>
@@ -2330,7 +2354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>6</v>
       </c>
@@ -2399,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>6</v>
       </c>
@@ -2468,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>6</v>
       </c>
@@ -2537,7 +2561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>6</v>
       </c>
@@ -2612,7 +2636,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>6</v>
       </c>
@@ -2690,7 +2714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>6</v>
       </c>
@@ -2771,7 +2795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>6</v>
       </c>
@@ -2840,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>6</v>
       </c>
@@ -2912,7 +2936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>6</v>
       </c>
@@ -2981,7 +3005,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>6</v>
       </c>
@@ -3053,7 +3077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>6</v>
       </c>
@@ -3122,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>6</v>
       </c>
@@ -3194,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>6</v>
       </c>
@@ -3269,7 +3293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -3341,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>6</v>
       </c>
@@ -3413,7 +3437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>6</v>
       </c>
@@ -3485,7 +3509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>6</v>
       </c>
@@ -3560,7 +3584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>6</v>
       </c>
@@ -3629,7 +3653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>6</v>
       </c>
@@ -3707,7 +3731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>6</v>
       </c>
@@ -3779,7 +3803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>6</v>
       </c>
@@ -3848,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>6</v>
       </c>
@@ -3917,7 +3941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>6</v>
       </c>
@@ -4007,7 +4031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>6</v>
       </c>
@@ -4082,7 +4106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>6</v>
       </c>
@@ -4157,7 +4181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>6</v>
       </c>
@@ -4235,7 +4259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>6</v>
       </c>
@@ -4307,7 +4331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>6</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>6</v>
       </c>
@@ -4451,7 +4475,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>6</v>
       </c>
@@ -4523,7 +4547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>6</v>
       </c>
@@ -4595,7 +4619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>6</v>
       </c>
@@ -4664,7 +4688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>6</v>
       </c>
@@ -4742,7 +4766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>6</v>
       </c>
@@ -4817,7 +4841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>6</v>
       </c>
@@ -4892,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>6</v>
       </c>
@@ -4967,7 +4991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>6</v>
       </c>
@@ -5045,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>6</v>
       </c>
@@ -5120,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>6</v>
       </c>
@@ -5186,7 +5210,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>6</v>
       </c>
@@ -5255,7 +5279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>6</v>
       </c>
@@ -5327,7 +5351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>6</v>
       </c>
@@ -5396,7 +5420,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>6</v>
       </c>
@@ -5468,7 +5492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>6</v>
       </c>
@@ -5540,7 +5564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>6</v>
       </c>
@@ -5609,7 +5633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>6</v>
       </c>
@@ -5678,7 +5702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>6</v>
       </c>
@@ -5753,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>6</v>
       </c>
@@ -5828,7 +5852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>6</v>
       </c>
@@ -5900,7 +5924,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>6</v>
       </c>
@@ -5975,7 +5999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>6</v>
       </c>
@@ -6050,7 +6074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>6</v>
       </c>
@@ -6119,7 +6143,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>6</v>
       </c>
@@ -6188,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>6</v>
       </c>
@@ -6266,7 +6290,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>6</v>
       </c>
@@ -6341,7 +6365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>6</v>
       </c>
@@ -6419,7 +6443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>6</v>
       </c>
@@ -6488,7 +6512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>6</v>
       </c>
@@ -6563,7 +6587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>6</v>
       </c>
@@ -6638,7 +6662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>6</v>
       </c>
@@ -6716,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>6</v>
       </c>
@@ -6794,7 +6818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>6</v>
       </c>
@@ -6875,7 +6899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>6</v>
       </c>
@@ -6944,7 +6968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>6</v>
       </c>
@@ -7028,7 +7052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>6</v>
       </c>
@@ -7100,7 +7124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>6</v>
       </c>
@@ -7172,7 +7196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>6</v>
       </c>
@@ -7247,7 +7271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>6</v>
       </c>
@@ -7322,7 +7346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>6</v>
       </c>
@@ -7394,7 +7418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>6</v>
       </c>
@@ -7472,7 +7496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>6</v>
       </c>
@@ -7541,7 +7565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>6</v>
       </c>
@@ -7616,7 +7640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>6</v>
       </c>
@@ -7691,7 +7715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>6</v>
       </c>
@@ -7772,7 +7796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>6</v>
       </c>
@@ -7841,7 +7865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>6</v>
       </c>
@@ -7913,7 +7937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>6</v>
       </c>
@@ -7982,13 +8006,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N101" s="2"/>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N102" s="2"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N103" s="2"/>
     </row>
   </sheetData>
@@ -8004,31 +8028,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA563366-8DA0-4A43-8949-852B034D9918}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q77" sqref="Q77:Q81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -8081,7 +8105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44723</v>
       </c>
@@ -8131,7 +8155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44723</v>
       </c>
@@ -8184,7 +8208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44723</v>
       </c>
@@ -8234,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44723</v>
       </c>
@@ -8284,7 +8308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44723</v>
       </c>
@@ -8334,7 +8358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44723</v>
       </c>
@@ -8387,7 +8411,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44724</v>
       </c>
@@ -8437,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44724</v>
       </c>
@@ -8487,7 +8511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44724</v>
       </c>
@@ -8537,7 +8561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44724</v>
       </c>
@@ -8587,7 +8611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44724</v>
       </c>
@@ -8637,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44724</v>
       </c>
@@ -8687,7 +8711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44724</v>
       </c>
@@ -8737,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44724</v>
       </c>
@@ -8787,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44724</v>
       </c>
@@ -8837,7 +8861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44724</v>
       </c>
@@ -8887,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44724</v>
       </c>
@@ -8937,7 +8961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44729</v>
       </c>
@@ -8987,7 +9011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44729</v>
       </c>
@@ -9037,7 +9061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44729</v>
       </c>
@@ -9087,7 +9111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44729</v>
       </c>
@@ -9137,7 +9161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44729</v>
       </c>
@@ -9187,7 +9211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44729</v>
       </c>
@@ -9237,7 +9261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44729</v>
       </c>
@@ -9287,7 +9311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44729</v>
       </c>
@@ -9337,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44729</v>
       </c>
@@ -9387,7 +9411,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44729</v>
       </c>
@@ -9437,7 +9461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44731</v>
       </c>
@@ -9487,7 +9511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44731</v>
       </c>
@@ -9537,7 +9561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44731</v>
       </c>
@@ -9587,7 +9611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44731</v>
       </c>
@@ -9637,7 +9661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44731</v>
       </c>
@@ -9687,7 +9711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44731</v>
       </c>
@@ -9737,7 +9761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44731</v>
       </c>
@@ -9787,7 +9811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44731</v>
       </c>
@@ -9837,7 +9861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44731</v>
       </c>
@@ -9887,7 +9911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44731</v>
       </c>
@@ -9937,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44731</v>
       </c>
@@ -9987,7 +10011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44731</v>
       </c>
@@ -10037,7 +10061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44731</v>
       </c>
@@ -10087,7 +10111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44731</v>
       </c>
@@ -10137,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44731</v>
       </c>
@@ -10187,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44731</v>
       </c>
@@ -10237,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44731</v>
       </c>
@@ -10287,7 +10311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44731</v>
       </c>
@@ -10340,7 +10364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44731</v>
       </c>
@@ -10390,7 +10414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44731</v>
       </c>
@@ -10440,7 +10464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44731</v>
       </c>
@@ -10490,7 +10514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44731</v>
       </c>
@@ -10540,7 +10564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44731</v>
       </c>
@@ -10590,7 +10614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44731</v>
       </c>
@@ -10640,7 +10664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44731</v>
       </c>
@@ -10690,7 +10714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44731</v>
       </c>
@@ -10740,7 +10764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44731</v>
       </c>
@@ -10790,7 +10814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44731</v>
       </c>
@@ -10840,7 +10864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44731</v>
       </c>
@@ -10890,7 +10914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44736</v>
       </c>
@@ -10940,7 +10964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44736</v>
       </c>
@@ -10990,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44736</v>
       </c>
@@ -11040,7 +11064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44736</v>
       </c>
@@ -11090,7 +11114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44736</v>
       </c>
@@ -11140,7 +11164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44736</v>
       </c>
@@ -11190,7 +11214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44736</v>
       </c>
@@ -11240,7 +11264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44736</v>
       </c>
@@ -11290,7 +11314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44736</v>
       </c>
@@ -11340,7 +11364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44736</v>
       </c>
@@ -11390,7 +11414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44736</v>
       </c>
@@ -11440,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44737</v>
       </c>
@@ -11490,7 +11514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44737</v>
       </c>
@@ -11540,7 +11564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44737</v>
       </c>
@@ -11590,7 +11614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44737</v>
       </c>
@@ -11640,7 +11664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44737</v>
       </c>
@@ -11690,7 +11714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44737</v>
       </c>
@@ -11740,7 +11764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44737</v>
       </c>
@@ -11790,7 +11814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44737</v>
       </c>
@@ -11840,7 +11864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44737</v>
       </c>
@@ -11890,7 +11914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44737</v>
       </c>
@@ -11940,7 +11964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44737</v>
       </c>
@@ -11990,7 +12014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44737</v>
       </c>
@@ -12040,7 +12064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44737</v>
       </c>
@@ -12090,7 +12114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44737</v>
       </c>
@@ -12140,7 +12164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44737</v>
       </c>
@@ -12190,7 +12214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44737</v>
       </c>
@@ -12240,7 +12264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44737</v>
       </c>
@@ -12290,7 +12314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44737</v>
       </c>
@@ -12340,7 +12364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44737</v>
       </c>
@@ -12393,7 +12417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44737</v>
       </c>
@@ -12443,7 +12467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44737</v>
       </c>
@@ -12493,7 +12517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44737</v>
       </c>
@@ -12543,7 +12567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44737</v>
       </c>
@@ -12593,7 +12617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44737</v>
       </c>
@@ -12643,7 +12667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44737</v>
       </c>
@@ -12693,7 +12717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44737</v>
       </c>
@@ -12743,7 +12767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44737</v>
       </c>
@@ -12793,7 +12817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44737</v>
       </c>
@@ -12843,7 +12867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44737</v>
       </c>
@@ -12893,7 +12917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44737</v>
       </c>
@@ -12943,7 +12967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44737</v>
       </c>
@@ -12993,7 +13017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44737</v>
       </c>
@@ -13057,18 +13081,18 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -13091,7 +13115,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -13114,7 +13138,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -13137,7 +13161,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -13160,7 +13184,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -13183,7 +13207,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -13206,7 +13230,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -13229,7 +13253,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -13252,7 +13276,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -13275,7 +13299,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -13298,7 +13322,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -13321,7 +13345,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -13344,7 +13368,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -13367,7 +13391,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -13390,7 +13414,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -13413,7 +13437,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -13436,7 +13460,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -13459,7 +13483,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -13482,7 +13506,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -13505,7 +13529,7 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -13528,7 +13552,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -13551,7 +13575,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -13574,7 +13598,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -13597,7 +13621,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -13620,7 +13644,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -13643,7 +13667,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -13662,7 +13686,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -13681,7 +13705,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -13700,7 +13724,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -13719,7 +13743,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -13738,7 +13762,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -13767,24 +13791,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5379496-B6C4-421B-9D7D-11C06426F583}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -13800,45 +13823,47 @@
       <c r="E1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4.13</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.5</v>
+      </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="5">
-        <v>4.13</v>
+        <v>4.17</v>
       </c>
       <c r="D3" s="9">
         <v>0.5</v>
@@ -13846,24 +13871,23 @@
       <c r="E3" s="5">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="5">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="D4" s="9">
         <v>0.25</v>
@@ -13871,24 +13895,23 @@
       <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="5">
-        <v>3.8</v>
+        <v>2.16</v>
       </c>
       <c r="D5" s="9">
         <v>0.25</v>
@@ -13896,24 +13919,23 @@
       <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="5"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="5">
-        <v>4.24</v>
+        <v>1.21</v>
       </c>
       <c r="D6" s="9">
         <v>0.5</v>
@@ -13921,170 +13943,165 @@
       <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="5">
-        <v>3.23</v>
+      <c r="C7" s="8">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D7" s="9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="5">
         <v>6</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="8">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="D8" s="9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="5">
         <v>7</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="5">
-        <v>4.8</v>
+        <v>3.4</v>
       </c>
       <c r="D9" s="9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E9" s="5">
         <v>8</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="5">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="D10" s="9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="5">
         <v>9</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="8">
-        <v>4.3</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4.18</v>
       </c>
       <c r="D11" s="9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E11" s="5">
         <v>10</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5">
         <v>11</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5">
-        <v>2.8</v>
+        <v>1.22</v>
       </c>
       <c r="D13" s="9">
         <v>0.5</v>
@@ -14092,24 +14109,23 @@
       <c r="E13" s="5">
         <v>12</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="5">
-        <v>1.1599999999999999</v>
+        <v>3.23</v>
       </c>
       <c r="D14" s="9">
         <v>0.25</v>
@@ -14117,112 +14133,115 @@
       <c r="E14" s="5">
         <v>13</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="5"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.25</v>
+      </c>
       <c r="E15" s="5">
         <v>14</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="5"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5">
         <v>15</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5">
         <v>16</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1.1000000000000001</v>
+        <v>47</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4.24</v>
       </c>
       <c r="D18" s="9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E18" s="5">
         <v>17</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
-        <v>1.1299999999999999</v>
+        <v>3.7</v>
       </c>
       <c r="D19" s="9">
         <v>0.25</v>
@@ -14230,74 +14249,69 @@
       <c r="E19" s="5">
         <v>18</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5">
+        <v>19</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="8">
-        <v>3.1</v>
-      </c>
-      <c r="D20" s="9">
+      <c r="C21" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D21" s="9">
         <v>0.25</v>
-      </c>
-      <c r="E20" s="5">
-        <v>19</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>17</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.5</v>
       </c>
       <c r="E21" s="5">
         <v>20</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="5">
-        <v>4.17</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4.3</v>
       </c>
       <c r="D22" s="9">
         <v>0.5</v>
@@ -14305,99 +14319,93 @@
       <c r="E22" s="5">
         <v>21</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="5"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0.5</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5">
         <v>22</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="5"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="5">
-        <v>2.16</v>
+        <v>2.14</v>
       </c>
       <c r="D24" s="9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="5">
         <v>23</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5">
-        <v>2.7</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="D25" s="9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E25" s="5">
         <v>24</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="5">
-        <v>3.4</v>
+        <v>1.6</v>
       </c>
       <c r="D26" s="9">
         <v>0.25</v>
@@ -14405,49 +14413,47 @@
       <c r="E26" s="5">
         <v>25</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="5">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="D27" s="9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="5">
         <v>26</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5">
-        <v>2.14</v>
+        <v>4.8</v>
       </c>
       <c r="D28" s="9">
         <v>0.5</v>
@@ -14455,24 +14461,23 @@
       <c r="E28" s="5">
         <v>27</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="5"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5">
-        <v>1.21</v>
+        <v>4.16</v>
       </c>
       <c r="D29" s="9">
         <v>0.5</v>
@@ -14480,24 +14485,23 @@
       <c r="E29" s="5">
         <v>28</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="5"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="5">
-        <v>4.18</v>
+        <v>3.8</v>
       </c>
       <c r="D30" s="9">
         <v>0.25</v>
@@ -14505,39 +14509,39 @@
       <c r="E30" s="5">
         <v>29</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="5"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>26</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5">
         <v>30</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
-    <sortCondition ref="E1:E31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
+    <sortCondition ref="E1:E32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editted that shit now I gotta read some shit
</commit_message>
<xml_diff>
--- a/round bald data.xlsx
+++ b/round bald data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Desktop\WCU\thesisschmesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonhi\OneDrive\Desktop\WCU\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3814063-BEA9-492B-91FD-F584F6E77329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70F6969-6360-41D8-B2B4-9386E053F5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="3" xr2:uid="{C93C8A9F-749A-4500-9DE3-023D8B4996BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="1" r:id="rId1"/>
@@ -263,12 +263,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,12 +281,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -744,13 +737,13 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>2022</v>
       </c>
       <c r="D2">
@@ -819,13 +812,13 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>11</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>2022</v>
       </c>
       <c r="D3">
@@ -894,13 +887,13 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>2022</v>
       </c>
       <c r="D4">
@@ -969,13 +962,13 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>11</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>2022</v>
       </c>
       <c r="D5">
@@ -1035,13 +1028,13 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>2022</v>
       </c>
       <c r="D6">
@@ -1113,13 +1106,13 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>11</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7">
@@ -1191,13 +1184,13 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>2022</v>
       </c>
       <c r="D8">
@@ -1263,13 +1256,13 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>2022</v>
       </c>
       <c r="D9">
@@ -1335,13 +1328,13 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>2022</v>
       </c>
       <c r="D10">
@@ -1410,13 +1403,13 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>12</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>2022</v>
       </c>
       <c r="D11">
@@ -1485,13 +1478,13 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>12</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>2022</v>
       </c>
       <c r="D12">
@@ -1554,13 +1547,13 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>6</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>2022</v>
       </c>
       <c r="D13">
@@ -1623,13 +1616,13 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>2022</v>
       </c>
       <c r="D14">
@@ -1695,13 +1688,13 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>6</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>2022</v>
       </c>
       <c r="D15">
@@ -1770,13 +1763,13 @@
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>6</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>2022</v>
       </c>
       <c r="D16">
@@ -1848,13 +1841,13 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>2022</v>
       </c>
       <c r="D17">
@@ -1923,13 +1916,13 @@
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>2022</v>
       </c>
       <c r="D18">
@@ -1995,13 +1988,13 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19">
         <v>6</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>17</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>2022</v>
       </c>
       <c r="D19">
@@ -2067,13 +2060,13 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>2022</v>
       </c>
       <c r="D20">
@@ -2139,13 +2132,13 @@
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21">
         <v>6</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>2022</v>
       </c>
       <c r="D21">
@@ -2211,13 +2204,13 @@
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <v>17</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>2022</v>
       </c>
       <c r="D22">
@@ -2283,13 +2276,13 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23">
         <v>6</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23">
         <v>17</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>2022</v>
       </c>
       <c r="D23">
@@ -2355,13 +2348,13 @@
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24">
         <v>6</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24">
         <v>17</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24">
         <v>2022</v>
       </c>
       <c r="D24">
@@ -2424,13 +2417,13 @@
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25">
         <v>17</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>2022</v>
       </c>
       <c r="D25">
@@ -2493,13 +2486,13 @@
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26">
         <v>17</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26">
         <v>2022</v>
       </c>
       <c r="D26">
@@ -2562,13 +2555,13 @@
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27">
         <v>6</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27">
         <v>17</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27">
         <v>2022</v>
       </c>
       <c r="D27">
@@ -2637,13 +2630,13 @@
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28">
         <v>6</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28">
         <v>17</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28">
         <v>2022</v>
       </c>
       <c r="D28">
@@ -2715,13 +2708,13 @@
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29">
         <v>6</v>
       </c>
-      <c r="B29" s="4">
-        <v>19</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="B29">
+        <v>19</v>
+      </c>
+      <c r="C29">
         <v>2022</v>
       </c>
       <c r="D29">
@@ -2796,13 +2789,13 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30">
         <v>6</v>
       </c>
-      <c r="B30" s="4">
-        <v>19</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="B30">
+        <v>19</v>
+      </c>
+      <c r="C30">
         <v>2022</v>
       </c>
       <c r="D30">
@@ -2865,13 +2858,13 @@
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31">
         <v>6</v>
       </c>
-      <c r="B31" s="4">
-        <v>19</v>
-      </c>
-      <c r="C31" s="4">
+      <c r="B31">
+        <v>19</v>
+      </c>
+      <c r="C31">
         <v>2022</v>
       </c>
       <c r="D31">
@@ -2937,13 +2930,13 @@
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32">
         <v>6</v>
       </c>
-      <c r="B32" s="4">
-        <v>19</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="B32">
+        <v>19</v>
+      </c>
+      <c r="C32">
         <v>2022</v>
       </c>
       <c r="D32">
@@ -3006,13 +2999,13 @@
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33">
         <v>6</v>
       </c>
-      <c r="B33" s="4">
-        <v>19</v>
-      </c>
-      <c r="C33" s="4">
+      <c r="B33">
+        <v>19</v>
+      </c>
+      <c r="C33">
         <v>2022</v>
       </c>
       <c r="D33">
@@ -3078,13 +3071,13 @@
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34">
         <v>6</v>
       </c>
-      <c r="B34" s="4">
-        <v>19</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="B34">
+        <v>19</v>
+      </c>
+      <c r="C34">
         <v>2022</v>
       </c>
       <c r="D34">
@@ -3147,13 +3140,13 @@
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35">
         <v>6</v>
       </c>
-      <c r="B35" s="4">
-        <v>19</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35">
         <v>2022</v>
       </c>
       <c r="D35">
@@ -3219,13 +3212,13 @@
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36">
         <v>6</v>
       </c>
-      <c r="B36" s="4">
-        <v>19</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="B36">
+        <v>19</v>
+      </c>
+      <c r="C36">
         <v>2022</v>
       </c>
       <c r="D36">
@@ -3294,13 +3287,13 @@
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37">
         <v>6</v>
       </c>
-      <c r="B37" s="4">
-        <v>19</v>
-      </c>
-      <c r="C37" s="4">
+      <c r="B37">
+        <v>19</v>
+      </c>
+      <c r="C37">
         <v>2022</v>
       </c>
       <c r="D37">
@@ -3366,13 +3359,13 @@
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38">
         <v>6</v>
       </c>
-      <c r="B38" s="4">
-        <v>19</v>
-      </c>
-      <c r="C38" s="4">
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38">
         <v>2022</v>
       </c>
       <c r="D38">
@@ -3438,13 +3431,13 @@
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39">
         <v>6</v>
       </c>
-      <c r="B39" s="4">
-        <v>19</v>
-      </c>
-      <c r="C39" s="4">
+      <c r="B39">
+        <v>19</v>
+      </c>
+      <c r="C39">
         <v>2022</v>
       </c>
       <c r="D39">
@@ -3510,13 +3503,13 @@
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40">
         <v>6</v>
       </c>
-      <c r="B40" s="4">
-        <v>19</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="B40">
+        <v>19</v>
+      </c>
+      <c r="C40">
         <v>2022</v>
       </c>
       <c r="D40">
@@ -3585,13 +3578,13 @@
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41">
         <v>6</v>
       </c>
-      <c r="B41" s="4">
-        <v>19</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="B41">
+        <v>19</v>
+      </c>
+      <c r="C41">
         <v>2022</v>
       </c>
       <c r="D41">
@@ -3654,13 +3647,13 @@
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42">
         <v>6</v>
       </c>
-      <c r="B42" s="4">
-        <v>19</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="B42">
+        <v>19</v>
+      </c>
+      <c r="C42">
         <v>2022</v>
       </c>
       <c r="D42">
@@ -3732,13 +3725,13 @@
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43">
         <v>6</v>
       </c>
-      <c r="B43" s="4">
-        <v>19</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="B43">
+        <v>19</v>
+      </c>
+      <c r="C43">
         <v>2022</v>
       </c>
       <c r="D43">
@@ -3804,13 +3797,13 @@
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44">
         <v>6</v>
       </c>
-      <c r="B44" s="4">
-        <v>19</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="B44">
+        <v>19</v>
+      </c>
+      <c r="C44">
         <v>2022</v>
       </c>
       <c r="D44">
@@ -3873,13 +3866,13 @@
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45">
         <v>6</v>
       </c>
-      <c r="B45" s="4">
-        <v>19</v>
-      </c>
-      <c r="C45" s="4">
+      <c r="B45">
+        <v>19</v>
+      </c>
+      <c r="C45">
         <v>2022</v>
       </c>
       <c r="D45">
@@ -3942,13 +3935,13 @@
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46">
         <v>6</v>
       </c>
-      <c r="B46" s="4">
-        <v>19</v>
-      </c>
-      <c r="C46" s="4">
+      <c r="B46">
+        <v>19</v>
+      </c>
+      <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46">
@@ -4032,13 +4025,13 @@
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47">
         <v>6</v>
       </c>
-      <c r="B47" s="4">
-        <v>19</v>
-      </c>
-      <c r="C47" s="4">
+      <c r="B47">
+        <v>19</v>
+      </c>
+      <c r="C47">
         <v>2022</v>
       </c>
       <c r="D47">
@@ -4107,13 +4100,13 @@
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48">
         <v>6</v>
       </c>
-      <c r="B48" s="4">
-        <v>19</v>
-      </c>
-      <c r="C48" s="4">
+      <c r="B48">
+        <v>19</v>
+      </c>
+      <c r="C48">
         <v>2022</v>
       </c>
       <c r="D48">
@@ -4182,13 +4175,13 @@
       </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49">
         <v>6</v>
       </c>
-      <c r="B49" s="4">
-        <v>19</v>
-      </c>
-      <c r="C49" s="4">
+      <c r="B49">
+        <v>19</v>
+      </c>
+      <c r="C49">
         <v>2022</v>
       </c>
       <c r="D49">
@@ -4260,13 +4253,13 @@
       </c>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50">
         <v>6</v>
       </c>
-      <c r="B50" s="4">
-        <v>19</v>
-      </c>
-      <c r="C50" s="4">
+      <c r="B50">
+        <v>19</v>
+      </c>
+      <c r="C50">
         <v>2022</v>
       </c>
       <c r="D50">
@@ -4332,13 +4325,13 @@
       </c>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51">
         <v>6</v>
       </c>
-      <c r="B51" s="4">
-        <v>19</v>
-      </c>
-      <c r="C51" s="4">
+      <c r="B51">
+        <v>19</v>
+      </c>
+      <c r="C51">
         <v>2022</v>
       </c>
       <c r="D51">
@@ -4407,13 +4400,13 @@
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52">
         <v>6</v>
       </c>
-      <c r="B52" s="4">
-        <v>19</v>
-      </c>
-      <c r="C52" s="4">
+      <c r="B52">
+        <v>19</v>
+      </c>
+      <c r="C52">
         <v>2022</v>
       </c>
       <c r="D52">
@@ -4476,13 +4469,13 @@
       </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53">
         <v>6</v>
       </c>
-      <c r="B53" s="4">
-        <v>19</v>
-      </c>
-      <c r="C53" s="4">
+      <c r="B53">
+        <v>19</v>
+      </c>
+      <c r="C53">
         <v>2022</v>
       </c>
       <c r="D53">
@@ -4548,13 +4541,13 @@
       </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54">
         <v>6</v>
       </c>
-      <c r="B54" s="4">
-        <v>19</v>
-      </c>
-      <c r="C54" s="4">
+      <c r="B54">
+        <v>19</v>
+      </c>
+      <c r="C54">
         <v>2022</v>
       </c>
       <c r="D54">
@@ -4620,13 +4613,13 @@
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55">
         <v>6</v>
       </c>
-      <c r="B55" s="4">
-        <v>19</v>
-      </c>
-      <c r="C55" s="4">
+      <c r="B55">
+        <v>19</v>
+      </c>
+      <c r="C55">
         <v>2022</v>
       </c>
       <c r="D55">
@@ -4689,13 +4682,13 @@
       </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56">
         <v>6</v>
       </c>
-      <c r="B56" s="4">
-        <v>19</v>
-      </c>
-      <c r="C56" s="4">
+      <c r="B56">
+        <v>19</v>
+      </c>
+      <c r="C56">
         <v>2022</v>
       </c>
       <c r="D56">
@@ -4767,13 +4760,13 @@
       </c>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57">
         <v>6</v>
       </c>
-      <c r="B57" s="4">
-        <v>19</v>
-      </c>
-      <c r="C57" s="4">
+      <c r="B57">
+        <v>19</v>
+      </c>
+      <c r="C57">
         <v>2022</v>
       </c>
       <c r="D57">
@@ -4842,13 +4835,13 @@
       </c>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="A58">
         <v>6</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58">
         <v>24</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58">
         <v>2022</v>
       </c>
       <c r="D58">
@@ -4917,13 +4910,13 @@
       </c>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59">
         <v>6</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59">
         <v>24</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59">
         <v>2022</v>
       </c>
       <c r="D59">
@@ -4992,13 +4985,13 @@
       </c>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="A60">
         <v>6</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60">
         <v>24</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60">
         <v>2022</v>
       </c>
       <c r="D60">
@@ -5070,13 +5063,13 @@
       </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="A61">
         <v>6</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61">
         <v>24</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61">
         <v>2022</v>
       </c>
       <c r="D61">
@@ -5145,13 +5138,13 @@
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62">
         <v>6</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62">
         <v>24</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62">
         <v>2022</v>
       </c>
       <c r="D62">
@@ -5211,13 +5204,13 @@
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63">
         <v>6</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63">
         <v>24</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63">
         <v>2022</v>
       </c>
       <c r="D63">
@@ -5280,13 +5273,13 @@
       </c>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="A64">
         <v>6</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64">
         <v>24</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64">
         <v>2022</v>
       </c>
       <c r="D64">
@@ -5352,13 +5345,13 @@
       </c>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65">
         <v>6</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65">
         <v>24</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65">
         <v>2022</v>
       </c>
       <c r="D65">
@@ -5421,13 +5414,13 @@
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66">
         <v>6</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66">
         <v>24</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66">
         <v>2022</v>
       </c>
       <c r="D66">
@@ -5493,13 +5486,13 @@
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67">
         <v>6</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67">
         <v>24</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67">
         <v>2022</v>
       </c>
       <c r="D67">
@@ -5565,13 +5558,13 @@
       </c>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68">
         <v>6</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68">
         <v>24</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68">
         <v>2022</v>
       </c>
       <c r="D68">
@@ -5634,13 +5627,13 @@
       </c>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="A69">
         <v>6</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69">
         <v>25</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69">
         <v>2022</v>
       </c>
       <c r="D69">
@@ -5703,13 +5696,13 @@
       </c>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70">
         <v>6</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70">
         <v>25</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70">
         <v>2022</v>
       </c>
       <c r="D70">
@@ -5778,13 +5771,13 @@
       </c>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71">
         <v>6</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71">
         <v>25</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71">
         <v>2022</v>
       </c>
       <c r="D71">
@@ -5853,13 +5846,13 @@
       </c>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="A72">
         <v>6</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72">
         <v>25</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72">
         <v>2022</v>
       </c>
       <c r="D72">
@@ -5925,13 +5918,13 @@
       </c>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="A73">
         <v>6</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73">
         <v>25</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73">
         <v>2022</v>
       </c>
       <c r="D73">
@@ -6000,13 +5993,13 @@
       </c>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74">
         <v>6</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74">
         <v>25</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74">
         <v>2022</v>
       </c>
       <c r="D74">
@@ -6075,13 +6068,13 @@
       </c>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="A75">
         <v>6</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75">
         <v>25</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75">
         <v>2022</v>
       </c>
       <c r="D75">
@@ -6144,13 +6137,13 @@
       </c>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="A76">
         <v>6</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76">
         <v>25</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76">
         <v>2022</v>
       </c>
       <c r="D76">
@@ -6213,13 +6206,13 @@
       </c>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="A77">
         <v>6</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77">
         <v>25</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77">
         <v>2022</v>
       </c>
       <c r="D77">
@@ -6291,13 +6284,13 @@
       </c>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="A78">
         <v>6</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78">
         <v>25</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78">
         <v>2022</v>
       </c>
       <c r="D78">
@@ -6366,13 +6359,13 @@
       </c>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="A79">
         <v>6</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79">
         <v>25</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79">
         <v>2022</v>
       </c>
       <c r="D79">
@@ -6444,13 +6437,13 @@
       </c>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="A80">
         <v>6</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80">
         <v>25</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80">
         <v>2022</v>
       </c>
       <c r="D80">
@@ -6513,13 +6506,13 @@
       </c>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="A81">
         <v>6</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81">
         <v>25</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81">
         <v>2022</v>
       </c>
       <c r="D81">
@@ -6588,13 +6581,13 @@
       </c>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="A82">
         <v>6</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82">
         <v>25</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82">
         <v>2022</v>
       </c>
       <c r="D82">
@@ -6663,13 +6656,13 @@
       </c>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="A83">
         <v>6</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83">
         <v>25</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83">
         <v>2022</v>
       </c>
       <c r="D83">
@@ -6741,13 +6734,13 @@
       </c>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="A84">
         <v>6</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B84">
         <v>25</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84">
         <v>2022</v>
       </c>
       <c r="D84">
@@ -6819,13 +6812,13 @@
       </c>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="A85">
         <v>6</v>
       </c>
-      <c r="B85" s="4">
+      <c r="B85">
         <v>25</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85">
         <v>2022</v>
       </c>
       <c r="D85">
@@ -6900,13 +6893,13 @@
       </c>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="A86">
         <v>6</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B86">
         <v>25</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86">
         <v>2022</v>
       </c>
       <c r="D86">
@@ -6969,13 +6962,13 @@
       </c>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="A87">
         <v>6</v>
       </c>
-      <c r="B87" s="4">
+      <c r="B87">
         <v>25</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87">
         <v>2022</v>
       </c>
       <c r="D87">
@@ -7053,13 +7046,13 @@
       </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="A88">
         <v>6</v>
       </c>
-      <c r="B88" s="4">
+      <c r="B88">
         <v>25</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88">
         <v>2022</v>
       </c>
       <c r="D88">
@@ -7125,13 +7118,13 @@
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="A89">
         <v>6</v>
       </c>
-      <c r="B89" s="4">
+      <c r="B89">
         <v>25</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89">
         <v>2022</v>
       </c>
       <c r="D89">
@@ -7197,13 +7190,13 @@
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="A90">
         <v>6</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B90">
         <v>25</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90">
         <v>2022</v>
       </c>
       <c r="D90">
@@ -7272,13 +7265,13 @@
       </c>
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="A91">
         <v>6</v>
       </c>
-      <c r="B91" s="4">
+      <c r="B91">
         <v>25</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91">
         <v>2022</v>
       </c>
       <c r="D91">
@@ -7347,13 +7340,13 @@
       </c>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="A92">
         <v>6</v>
       </c>
-      <c r="B92" s="4">
+      <c r="B92">
         <v>25</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92">
         <v>2022</v>
       </c>
       <c r="D92">
@@ -7419,13 +7412,13 @@
       </c>
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="A93">
         <v>6</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93">
         <v>25</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93">
         <v>2022</v>
       </c>
       <c r="D93">
@@ -7497,13 +7490,13 @@
       </c>
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="A94">
         <v>6</v>
       </c>
-      <c r="B94" s="4">
+      <c r="B94">
         <v>25</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94">
         <v>2022</v>
       </c>
       <c r="D94">
@@ -7566,13 +7559,13 @@
       </c>
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="A95">
         <v>6</v>
       </c>
-      <c r="B95" s="4">
+      <c r="B95">
         <v>25</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95">
         <v>2022</v>
       </c>
       <c r="D95">
@@ -7641,13 +7634,13 @@
       </c>
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+      <c r="A96">
         <v>6</v>
       </c>
-      <c r="B96" s="4">
+      <c r="B96">
         <v>25</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96">
         <v>2022</v>
       </c>
       <c r="D96">
@@ -7716,13 +7709,13 @@
       </c>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
+      <c r="A97">
         <v>6</v>
       </c>
-      <c r="B97" s="4">
+      <c r="B97">
         <v>25</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97">
         <v>2022</v>
       </c>
       <c r="D97">
@@ -7797,13 +7790,13 @@
       </c>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+      <c r="A98">
         <v>6</v>
       </c>
-      <c r="B98" s="4">
+      <c r="B98">
         <v>25</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98">
         <v>2022</v>
       </c>
       <c r="D98">
@@ -7866,13 +7859,13 @@
       </c>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="A99">
         <v>6</v>
       </c>
-      <c r="B99" s="4">
+      <c r="B99">
         <v>25</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99">
         <v>2022</v>
       </c>
       <c r="D99">
@@ -7938,13 +7931,13 @@
       </c>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+      <c r="A100">
         <v>6</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B100">
         <v>25</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C100">
         <v>2022</v>
       </c>
       <c r="D100">
@@ -13096,690 +13089,690 @@
       <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1.21</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.5</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1.22</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.5</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2.14</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.5</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.5</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4.24</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.5</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>4.3</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.5</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.25</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1.1599999999999999</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.25</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>2.16</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.25</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3.8</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.25</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>3.1</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0.25</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>3.23</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>0.25</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>2.7</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>0.5</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>2.8</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>0.5</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>4.8</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>0.5</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>4.13</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>0.5</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>4.16</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>0.5</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>4.17</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>0.5</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>1.6</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>0.25</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>1.7</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>0.25</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>0.25</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>3.4</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>0.25</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>3.7</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>0.25</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>4.18</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>0.25</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
@@ -13794,7 +13787,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:E31"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13803,7 +13796,7 @@
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13811,733 +13804,733 @@
       <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.16</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C4" s="4">
         <v>3.8</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D4" s="8">
         <v>0.25</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="4">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C8" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D8" s="8">
         <v>0.5</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E8" s="4">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="4">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4.24</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="4">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>16</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>2</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="B18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.22</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>17</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4.18</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="4">
+        <v>19</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="4">
+        <v>20</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.14</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>21</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="4">
+        <v>22</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>12</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3.23</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E24" s="4">
+        <v>23</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>30</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <v>24</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4">
+        <v>4.17</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="4">
+        <v>25</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>16</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4.13</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="4">
+        <v>26</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E28" s="4">
+        <v>27</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>17</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="4">
+        <v>4.16</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="4">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="F29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
-        <v>3</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4">
+        <v>29</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="5">
-        <v>1.21</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>4</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>24</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4.18</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C31" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D31" s="8">
         <v>0.25</v>
       </c>
-      <c r="E6" s="5">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="5">
-        <v>6</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="5">
-        <v>7</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="5">
-        <v>4.8</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="5">
-        <v>8</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>23</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E10" s="5">
-        <v>9</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="5">
-        <v>10</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2.14</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="5">
-        <v>11</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="5">
-        <v>4.13</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="5">
-        <v>12</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="5">
-        <v>3.23</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="5">
-        <v>13</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="E31" s="4">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5">
-        <v>14</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>11</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="8">
-        <v>3.1</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E16" s="5">
-        <v>15</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>16</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>26</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5">
-        <v>17</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5">
-        <v>18</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>7</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="5">
-        <v>19</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>18</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="5">
-        <v>20</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>29</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
-        <v>21</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E23" s="5">
-        <v>22</v>
-      </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>27</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
-        <v>23</v>
-      </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>2</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="5">
-        <v>24</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>5</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5">
-        <v>4.24</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E26" s="5">
-        <v>25</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>20</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E27" s="5">
-        <v>26</v>
-      </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>8</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E28" s="5">
-        <v>27</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>19</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="D29" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E29" s="5">
-        <v>28</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>13</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E30" s="5">
-        <v>29</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>9</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="5">
-        <v>2.16</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E31" s="5">
-        <v>30</v>
-      </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">

</xml_diff>